<commit_message>
Updated Unit Test For Week 9
</commit_message>
<xml_diff>
--- a/UnitTestFile/UniTests.xlsx
+++ b/UnitTestFile/UniTests.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311EA966-57E1-4B4A-A734-9FDB9F5E3688}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBB1132-E87E-4A3E-8B0C-C0111F19DE32}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2953" uniqueCount="102">
   <si>
     <t>White Rook</t>
   </si>
@@ -221,6 +221,111 @@
   </si>
   <si>
     <t>D5</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>FIRST TURN</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>F6</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>F7</t>
+  </si>
+  <si>
+    <t>G8</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>G5</t>
+  </si>
+  <si>
+    <t>H5</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D1</t>
   </si>
 </sst>
 </file>
@@ -554,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:Y159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="AA32" sqref="AA32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,6 +674,7 @@
     <col min="15" max="15" width="14.5703125" customWidth="1"/>
     <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.28515625" customWidth="1"/>
     <col min="21" max="21" width="11.7109375" customWidth="1"/>
     <col min="22" max="22" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15.7109375" bestFit="1" customWidth="1"/>
@@ -694,11 +800,18 @@
       </c>
       <c r="S5" s="1"/>
       <c r="U5" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="V5" t="s">
         <v>66</v>
       </c>
+      <c r="W5" t="s">
+        <v>67</v>
+      </c>
+      <c r="X5" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y5" s="1"/>
     </row>
     <row r="6" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
@@ -734,6 +847,19 @@
         <v>57</v>
       </c>
       <c r="S6" s="1"/>
+      <c r="U6" t="s">
+        <v>22</v>
+      </c>
+      <c r="V6" t="s">
+        <v>66</v>
+      </c>
+      <c r="W6" t="s">
+        <v>64</v>
+      </c>
+      <c r="X6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y6" s="1"/>
     </row>
     <row r="7" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
@@ -769,6 +895,19 @@
         <v>57</v>
       </c>
       <c r="S7" s="1"/>
+      <c r="U7" t="s">
+        <v>22</v>
+      </c>
+      <c r="V7" t="s">
+        <v>66</v>
+      </c>
+      <c r="W7" t="s">
+        <v>71</v>
+      </c>
+      <c r="X7" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y7" s="1"/>
     </row>
     <row r="8" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
@@ -804,6 +943,19 @@
         <v>57</v>
       </c>
       <c r="S8" s="1"/>
+      <c r="U8" t="s">
+        <v>22</v>
+      </c>
+      <c r="V8" t="s">
+        <v>66</v>
+      </c>
+      <c r="W8" t="s">
+        <v>72</v>
+      </c>
+      <c r="X8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y8" s="1"/>
     </row>
     <row r="9" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
@@ -839,6 +991,19 @@
         <v>57</v>
       </c>
       <c r="S9" s="1"/>
+      <c r="U9" t="s">
+        <v>22</v>
+      </c>
+      <c r="V9" t="s">
+        <v>66</v>
+      </c>
+      <c r="W9" t="s">
+        <v>73</v>
+      </c>
+      <c r="X9" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y9" s="1"/>
     </row>
     <row r="10" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
@@ -874,6 +1039,19 @@
         <v>57</v>
       </c>
       <c r="S10" s="1"/>
+      <c r="U10" t="s">
+        <v>22</v>
+      </c>
+      <c r="V10" t="s">
+        <v>66</v>
+      </c>
+      <c r="W10" t="s">
+        <v>68</v>
+      </c>
+      <c r="X10" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y10" s="1"/>
     </row>
     <row r="11" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
@@ -909,6 +1087,19 @@
         <v>57</v>
       </c>
       <c r="S11" s="1"/>
+      <c r="U11" t="s">
+        <v>22</v>
+      </c>
+      <c r="V11" t="s">
+        <v>66</v>
+      </c>
+      <c r="W11" t="s">
+        <v>74</v>
+      </c>
+      <c r="X11" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y11" s="1"/>
     </row>
     <row r="12" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
@@ -944,6 +1135,19 @@
         <v>57</v>
       </c>
       <c r="S12" s="1"/>
+      <c r="U12" t="s">
+        <v>22</v>
+      </c>
+      <c r="V12" t="s">
+        <v>66</v>
+      </c>
+      <c r="W12" t="s">
+        <v>75</v>
+      </c>
+      <c r="X12" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y12" s="1"/>
     </row>
     <row r="13" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
@@ -1014,6 +1218,19 @@
         <v>57</v>
       </c>
       <c r="S14" s="1"/>
+      <c r="U14" t="s">
+        <v>24</v>
+      </c>
+      <c r="V14" t="s">
+        <v>66</v>
+      </c>
+      <c r="W14" t="s">
+        <v>75</v>
+      </c>
+      <c r="X14" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y14" s="1"/>
     </row>
     <row r="15" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
@@ -1049,6 +1266,22 @@
         <v>57</v>
       </c>
       <c r="S15" s="1"/>
+      <c r="T15" t="s">
+        <v>76</v>
+      </c>
+      <c r="U15" t="s">
+        <v>24</v>
+      </c>
+      <c r="V15" t="s">
+        <v>66</v>
+      </c>
+      <c r="W15" t="s">
+        <v>77</v>
+      </c>
+      <c r="X15" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y15" s="1"/>
     </row>
     <row r="16" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
@@ -1085,7 +1318,7 @@
       </c>
       <c r="S16" s="1"/>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>24</v>
       </c>
@@ -1093,8 +1326,21 @@
         <v>17</v>
       </c>
       <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="U17" t="s">
+        <v>20</v>
+      </c>
+      <c r="V17" t="s">
+        <v>66</v>
+      </c>
+      <c r="W17" t="s">
+        <v>78</v>
+      </c>
+      <c r="X17" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y17" s="1"/>
+    </row>
+    <row r="18" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>24</v>
       </c>
@@ -1115,8 +1361,21 @@
         <v>56</v>
       </c>
       <c r="L18" s="1"/>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="U18" t="s">
+        <v>20</v>
+      </c>
+      <c r="V18" t="s">
+        <v>66</v>
+      </c>
+      <c r="W18" t="s">
+        <v>79</v>
+      </c>
+      <c r="X18" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y18" s="1"/>
+    </row>
+    <row r="19" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>24</v>
       </c>
@@ -1137,8 +1396,21 @@
         <v>56</v>
       </c>
       <c r="L19" s="1"/>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="U19" t="s">
+        <v>20</v>
+      </c>
+      <c r="V19" t="s">
+        <v>66</v>
+      </c>
+      <c r="W19" t="s">
+        <v>80</v>
+      </c>
+      <c r="X19" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y19" s="1"/>
+    </row>
+    <row r="20" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>24</v>
       </c>
@@ -1159,8 +1431,21 @@
         <v>56</v>
       </c>
       <c r="L20" s="1"/>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="U20" t="s">
+        <v>20</v>
+      </c>
+      <c r="V20" t="s">
+        <v>66</v>
+      </c>
+      <c r="W20" t="s">
+        <v>81</v>
+      </c>
+      <c r="X20" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y20" s="1"/>
+    </row>
+    <row r="21" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>25</v>
       </c>
@@ -1181,8 +1466,21 @@
         <v>56</v>
       </c>
       <c r="L21" s="1"/>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="U21" t="s">
+        <v>20</v>
+      </c>
+      <c r="V21" t="s">
+        <v>66</v>
+      </c>
+      <c r="W21" t="s">
+        <v>82</v>
+      </c>
+      <c r="X21" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y21" s="1"/>
+    </row>
+    <row r="22" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>25</v>
       </c>
@@ -1203,8 +1501,21 @@
         <v>56</v>
       </c>
       <c r="L22" s="1"/>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="U22" t="s">
+        <v>20</v>
+      </c>
+      <c r="V22" t="s">
+        <v>66</v>
+      </c>
+      <c r="W22" t="s">
+        <v>83</v>
+      </c>
+      <c r="X22" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y22" s="1"/>
+    </row>
+    <row r="23" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>42</v>
       </c>
@@ -1225,8 +1536,21 @@
         <v>56</v>
       </c>
       <c r="L23" s="1"/>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="U23" t="s">
+        <v>20</v>
+      </c>
+      <c r="V23" t="s">
+        <v>66</v>
+      </c>
+      <c r="W23" t="s">
+        <v>84</v>
+      </c>
+      <c r="X23" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y23" s="1"/>
+    </row>
+    <row r="24" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>42</v>
       </c>
@@ -1247,8 +1571,21 @@
         <v>57</v>
       </c>
       <c r="L24" s="1"/>
-    </row>
-    <row r="25" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="U24" t="s">
+        <v>20</v>
+      </c>
+      <c r="V24" t="s">
+        <v>66</v>
+      </c>
+      <c r="W24" t="s">
+        <v>85</v>
+      </c>
+      <c r="X24" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y24" s="1"/>
+    </row>
+    <row r="25" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>43</v>
       </c>
@@ -1270,7 +1607,7 @@
       </c>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>43</v>
       </c>
@@ -1291,8 +1628,21 @@
         <v>57</v>
       </c>
       <c r="L26" s="1"/>
-    </row>
-    <row r="27" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="U26" t="s">
+        <v>21</v>
+      </c>
+      <c r="V26" t="s">
+        <v>66</v>
+      </c>
+      <c r="W26" t="s">
+        <v>74</v>
+      </c>
+      <c r="X26" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y26" s="1"/>
+    </row>
+    <row r="27" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>44</v>
       </c>
@@ -1313,8 +1663,21 @@
         <v>57</v>
       </c>
       <c r="L27" s="1"/>
-    </row>
-    <row r="28" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="U27" t="s">
+        <v>21</v>
+      </c>
+      <c r="V27" t="s">
+        <v>66</v>
+      </c>
+      <c r="W27" t="s">
+        <v>86</v>
+      </c>
+      <c r="X27" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y27" s="1"/>
+    </row>
+    <row r="28" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>45</v>
       </c>
@@ -1335,8 +1698,21 @@
         <v>57</v>
       </c>
       <c r="L28" s="1"/>
-    </row>
-    <row r="29" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="U28" t="s">
+        <v>21</v>
+      </c>
+      <c r="V28" t="s">
+        <v>66</v>
+      </c>
+      <c r="W28" t="s">
+        <v>87</v>
+      </c>
+      <c r="X28" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y28" s="1"/>
+    </row>
+    <row r="29" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>46</v>
       </c>
@@ -1357,8 +1733,21 @@
         <v>57</v>
       </c>
       <c r="L29" s="1"/>
-    </row>
-    <row r="30" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="U29" t="s">
+        <v>21</v>
+      </c>
+      <c r="V29" t="s">
+        <v>66</v>
+      </c>
+      <c r="W29" t="s">
+        <v>73</v>
+      </c>
+      <c r="X29" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y29" s="1"/>
+    </row>
+    <row r="30" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>46</v>
       </c>
@@ -1366,8 +1755,21 @@
         <v>35</v>
       </c>
       <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="U30" t="s">
+        <v>21</v>
+      </c>
+      <c r="V30" t="s">
+        <v>66</v>
+      </c>
+      <c r="W30" t="s">
+        <v>88</v>
+      </c>
+      <c r="X30" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y30" s="1"/>
+    </row>
+    <row r="31" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>46</v>
       </c>
@@ -1388,8 +1790,21 @@
         <v>56</v>
       </c>
       <c r="L31" s="1"/>
-    </row>
-    <row r="32" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="U31" t="s">
+        <v>21</v>
+      </c>
+      <c r="V31" t="s">
+        <v>66</v>
+      </c>
+      <c r="W31" t="s">
+        <v>89</v>
+      </c>
+      <c r="X31" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y31" s="1"/>
+    </row>
+    <row r="32" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>46</v>
       </c>
@@ -1410,8 +1825,21 @@
         <v>56</v>
       </c>
       <c r="L32" s="1"/>
-    </row>
-    <row r="33" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="U32" t="s">
+        <v>21</v>
+      </c>
+      <c r="V32" t="s">
+        <v>66</v>
+      </c>
+      <c r="W32" t="s">
+        <v>71</v>
+      </c>
+      <c r="X32" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y32" s="1"/>
+    </row>
+    <row r="33" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>46</v>
       </c>
@@ -1432,8 +1860,21 @@
         <v>56</v>
       </c>
       <c r="L33" s="1"/>
-    </row>
-    <row r="34" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="U33" t="s">
+        <v>21</v>
+      </c>
+      <c r="V33" t="s">
+        <v>66</v>
+      </c>
+      <c r="W33" t="s">
+        <v>92</v>
+      </c>
+      <c r="X33" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y33" s="1"/>
+    </row>
+    <row r="34" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>46</v>
       </c>
@@ -1454,8 +1895,21 @@
         <v>56</v>
       </c>
       <c r="L34" s="1"/>
-    </row>
-    <row r="35" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="U34" t="s">
+        <v>21</v>
+      </c>
+      <c r="V34" t="s">
+        <v>66</v>
+      </c>
+      <c r="W34" t="s">
+        <v>91</v>
+      </c>
+      <c r="X34" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y34" s="1"/>
+    </row>
+    <row r="35" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>46</v>
       </c>
@@ -1476,8 +1930,21 @@
         <v>56</v>
       </c>
       <c r="L35" s="1"/>
-    </row>
-    <row r="36" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="U35" t="s">
+        <v>21</v>
+      </c>
+      <c r="V35" t="s">
+        <v>66</v>
+      </c>
+      <c r="W35" t="s">
+        <v>93</v>
+      </c>
+      <c r="X35" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y35" s="1"/>
+    </row>
+    <row r="36" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>46</v>
       </c>
@@ -1498,8 +1965,21 @@
         <v>56</v>
       </c>
       <c r="L36" s="1"/>
-    </row>
-    <row r="37" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="U36" t="s">
+        <v>21</v>
+      </c>
+      <c r="V36" t="s">
+        <v>66</v>
+      </c>
+      <c r="W36" t="s">
+        <v>64</v>
+      </c>
+      <c r="X36" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y36" s="1"/>
+    </row>
+    <row r="37" spans="3:25" x14ac:dyDescent="0.25">
       <c r="H37" t="s">
         <v>54</v>
       </c>
@@ -1513,8 +1993,21 @@
         <v>57</v>
       </c>
       <c r="L37" s="1"/>
-    </row>
-    <row r="38" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="U37" t="s">
+        <v>21</v>
+      </c>
+      <c r="V37" t="s">
+        <v>66</v>
+      </c>
+      <c r="W37" t="s">
+        <v>94</v>
+      </c>
+      <c r="X37" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y37" s="1"/>
+    </row>
+    <row r="38" spans="3:25" x14ac:dyDescent="0.25">
       <c r="H38" t="s">
         <v>54</v>
       </c>
@@ -1528,8 +2021,21 @@
         <v>57</v>
       </c>
       <c r="L38" s="1"/>
-    </row>
-    <row r="39" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="U38" t="s">
+        <v>21</v>
+      </c>
+      <c r="V38" t="s">
+        <v>66</v>
+      </c>
+      <c r="W38" t="s">
+        <v>95</v>
+      </c>
+      <c r="X38" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y38" s="1"/>
+    </row>
+    <row r="39" spans="3:25" x14ac:dyDescent="0.25">
       <c r="H39" t="s">
         <v>54</v>
       </c>
@@ -1544,7 +2050,7 @@
       </c>
       <c r="L39" s="1"/>
     </row>
-    <row r="40" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:25" x14ac:dyDescent="0.25">
       <c r="H40" t="s">
         <v>54</v>
       </c>
@@ -1558,8 +2064,21 @@
         <v>57</v>
       </c>
       <c r="L40" s="1"/>
-    </row>
-    <row r="41" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="U40" t="s">
+        <v>0</v>
+      </c>
+      <c r="V40" t="s">
+        <v>66</v>
+      </c>
+      <c r="W40" t="s">
+        <v>75</v>
+      </c>
+      <c r="X40" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y40" s="1"/>
+    </row>
+    <row r="41" spans="3:25" x14ac:dyDescent="0.25">
       <c r="H41" t="s">
         <v>54</v>
       </c>
@@ -1573,8 +2092,21 @@
         <v>57</v>
       </c>
       <c r="L41" s="1"/>
-    </row>
-    <row r="42" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="U41" t="s">
+        <v>0</v>
+      </c>
+      <c r="V41" t="s">
+        <v>66</v>
+      </c>
+      <c r="W41" t="s">
+        <v>77</v>
+      </c>
+      <c r="X41" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y41" s="1"/>
+    </row>
+    <row r="42" spans="3:25" x14ac:dyDescent="0.25">
       <c r="H42" t="s">
         <v>54</v>
       </c>
@@ -1588,8 +2120,36 @@
         <v>57</v>
       </c>
       <c r="L42" s="1"/>
-    </row>
-    <row r="44" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="U42" t="s">
+        <v>0</v>
+      </c>
+      <c r="V42" t="s">
+        <v>66</v>
+      </c>
+      <c r="W42" t="s">
+        <v>96</v>
+      </c>
+      <c r="X42" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y42" s="1"/>
+    </row>
+    <row r="43" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="U43" t="s">
+        <v>0</v>
+      </c>
+      <c r="V43" t="s">
+        <v>66</v>
+      </c>
+      <c r="W43" t="s">
+        <v>72</v>
+      </c>
+      <c r="X43" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y43" s="1"/>
+    </row>
+    <row r="44" spans="3:25" x14ac:dyDescent="0.25">
       <c r="H44" t="s">
         <v>21</v>
       </c>
@@ -1603,8 +2163,21 @@
         <v>56</v>
       </c>
       <c r="L44" s="1"/>
-    </row>
-    <row r="45" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="U44" t="s">
+        <v>0</v>
+      </c>
+      <c r="V44" t="s">
+        <v>66</v>
+      </c>
+      <c r="W44" t="s">
+        <v>97</v>
+      </c>
+      <c r="X44" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y44" s="1"/>
+    </row>
+    <row r="45" spans="3:25" x14ac:dyDescent="0.25">
       <c r="H45" t="s">
         <v>21</v>
       </c>
@@ -1618,8 +2191,21 @@
         <v>56</v>
       </c>
       <c r="L45" s="1"/>
-    </row>
-    <row r="46" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="U45" t="s">
+        <v>0</v>
+      </c>
+      <c r="V45" t="s">
+        <v>66</v>
+      </c>
+      <c r="W45" t="s">
+        <v>98</v>
+      </c>
+      <c r="X45" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y45" s="1"/>
+    </row>
+    <row r="46" spans="3:25" x14ac:dyDescent="0.25">
       <c r="H46" t="s">
         <v>21</v>
       </c>
@@ -1633,8 +2219,21 @@
         <v>56</v>
       </c>
       <c r="L46" s="1"/>
-    </row>
-    <row r="47" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="U46" t="s">
+        <v>0</v>
+      </c>
+      <c r="V46" t="s">
+        <v>66</v>
+      </c>
+      <c r="W46" t="s">
+        <v>99</v>
+      </c>
+      <c r="X46" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y46" s="1"/>
+    </row>
+    <row r="47" spans="3:25" x14ac:dyDescent="0.25">
       <c r="H47" t="s">
         <v>21</v>
       </c>
@@ -1648,8 +2247,21 @@
         <v>56</v>
       </c>
       <c r="L47" s="1"/>
-    </row>
-    <row r="48" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="U47" t="s">
+        <v>0</v>
+      </c>
+      <c r="V47" t="s">
+        <v>66</v>
+      </c>
+      <c r="W47" t="s">
+        <v>68</v>
+      </c>
+      <c r="X47" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y47" s="1"/>
+    </row>
+    <row r="48" spans="3:25" x14ac:dyDescent="0.25">
       <c r="H48" t="s">
         <v>21</v>
       </c>
@@ -1663,8 +2275,21 @@
         <v>56</v>
       </c>
       <c r="L48" s="1"/>
-    </row>
-    <row r="49" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U48" t="s">
+        <v>0</v>
+      </c>
+      <c r="V48" t="s">
+        <v>66</v>
+      </c>
+      <c r="W48" t="s">
+        <v>69</v>
+      </c>
+      <c r="X48" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y48" s="1"/>
+    </row>
+    <row r="49" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H49" t="s">
         <v>21</v>
       </c>
@@ -1678,8 +2303,21 @@
         <v>56</v>
       </c>
       <c r="L49" s="1"/>
-    </row>
-    <row r="50" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U49" t="s">
+        <v>0</v>
+      </c>
+      <c r="V49" t="s">
+        <v>66</v>
+      </c>
+      <c r="W49" t="s">
+        <v>70</v>
+      </c>
+      <c r="X49" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y49" s="1"/>
+    </row>
+    <row r="50" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H50" t="s">
         <v>21</v>
       </c>
@@ -1693,8 +2331,21 @@
         <v>57</v>
       </c>
       <c r="L50" s="1"/>
-    </row>
-    <row r="51" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U50" t="s">
+        <v>0</v>
+      </c>
+      <c r="V50" t="s">
+        <v>66</v>
+      </c>
+      <c r="W50" t="s">
+        <v>67</v>
+      </c>
+      <c r="X50" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y50" s="1"/>
+    </row>
+    <row r="51" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H51" t="s">
         <v>21</v>
       </c>
@@ -1708,8 +2359,21 @@
         <v>57</v>
       </c>
       <c r="L51" s="1"/>
-    </row>
-    <row r="52" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U51" t="s">
+        <v>0</v>
+      </c>
+      <c r="V51" t="s">
+        <v>66</v>
+      </c>
+      <c r="W51" t="s">
+        <v>90</v>
+      </c>
+      <c r="X51" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y51" s="1"/>
+    </row>
+    <row r="52" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H52" t="s">
         <v>21</v>
       </c>
@@ -1723,8 +2387,21 @@
         <v>57</v>
       </c>
       <c r="L52" s="1"/>
-    </row>
-    <row r="53" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U52" t="s">
+        <v>0</v>
+      </c>
+      <c r="V52" t="s">
+        <v>66</v>
+      </c>
+      <c r="W52" t="s">
+        <v>100</v>
+      </c>
+      <c r="X52" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y52" s="1"/>
+    </row>
+    <row r="53" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H53" t="s">
         <v>21</v>
       </c>
@@ -1738,8 +2415,21 @@
         <v>57</v>
       </c>
       <c r="L53" s="1"/>
-    </row>
-    <row r="54" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U53" t="s">
+        <v>0</v>
+      </c>
+      <c r="V53" t="s">
+        <v>66</v>
+      </c>
+      <c r="W53" t="s">
+        <v>101</v>
+      </c>
+      <c r="X53" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y53" s="1"/>
+    </row>
+    <row r="54" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H54" t="s">
         <v>21</v>
       </c>
@@ -1754,7 +2444,7 @@
       </c>
       <c r="L54" s="1"/>
     </row>
-    <row r="55" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H55" t="s">
         <v>21</v>
       </c>
@@ -1768,8 +2458,36 @@
         <v>57</v>
       </c>
       <c r="L55" s="1"/>
-    </row>
-    <row r="57" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U55" t="s">
+        <v>23</v>
+      </c>
+      <c r="V55" t="s">
+        <v>66</v>
+      </c>
+      <c r="W55" t="s">
+        <v>75</v>
+      </c>
+      <c r="X55" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y55" s="1"/>
+    </row>
+    <row r="56" spans="8:25" x14ac:dyDescent="0.25">
+      <c r="U56" t="s">
+        <v>23</v>
+      </c>
+      <c r="V56" t="s">
+        <v>66</v>
+      </c>
+      <c r="W56" t="s">
+        <v>77</v>
+      </c>
+      <c r="X56" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y56" s="1"/>
+    </row>
+    <row r="57" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H57" t="s">
         <v>22</v>
       </c>
@@ -1783,8 +2501,21 @@
         <v>56</v>
       </c>
       <c r="L57" s="1"/>
-    </row>
-    <row r="58" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U57" t="s">
+        <v>23</v>
+      </c>
+      <c r="V57" t="s">
+        <v>66</v>
+      </c>
+      <c r="W57" t="s">
+        <v>96</v>
+      </c>
+      <c r="X57" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y57" s="1"/>
+    </row>
+    <row r="58" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H58" t="s">
         <v>22</v>
       </c>
@@ -1798,8 +2529,21 @@
         <v>56</v>
       </c>
       <c r="L58" s="1"/>
-    </row>
-    <row r="59" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U58" t="s">
+        <v>23</v>
+      </c>
+      <c r="V58" t="s">
+        <v>66</v>
+      </c>
+      <c r="W58" t="s">
+        <v>72</v>
+      </c>
+      <c r="X58" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y58" s="1"/>
+    </row>
+    <row r="59" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H59" t="s">
         <v>22</v>
       </c>
@@ -1813,8 +2557,21 @@
         <v>56</v>
       </c>
       <c r="L59" s="1"/>
-    </row>
-    <row r="60" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U59" t="s">
+        <v>23</v>
+      </c>
+      <c r="V59" t="s">
+        <v>66</v>
+      </c>
+      <c r="W59" t="s">
+        <v>97</v>
+      </c>
+      <c r="X59" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y59" s="1"/>
+    </row>
+    <row r="60" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H60" t="s">
         <v>22</v>
       </c>
@@ -1828,8 +2585,21 @@
         <v>56</v>
       </c>
       <c r="L60" s="1"/>
-    </row>
-    <row r="61" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U60" t="s">
+        <v>23</v>
+      </c>
+      <c r="V60" t="s">
+        <v>66</v>
+      </c>
+      <c r="W60" t="s">
+        <v>98</v>
+      </c>
+      <c r="X60" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y60" s="1"/>
+    </row>
+    <row r="61" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H61" t="s">
         <v>22</v>
       </c>
@@ -1843,8 +2613,21 @@
         <v>56</v>
       </c>
       <c r="L61" s="1"/>
-    </row>
-    <row r="62" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U61" t="s">
+        <v>23</v>
+      </c>
+      <c r="V61" t="s">
+        <v>66</v>
+      </c>
+      <c r="W61" t="s">
+        <v>99</v>
+      </c>
+      <c r="X61" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y61" s="1"/>
+    </row>
+    <row r="62" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H62" t="s">
         <v>22</v>
       </c>
@@ -1858,8 +2641,21 @@
         <v>56</v>
       </c>
       <c r="L62" s="1"/>
-    </row>
-    <row r="63" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U62" t="s">
+        <v>23</v>
+      </c>
+      <c r="V62" t="s">
+        <v>66</v>
+      </c>
+      <c r="W62" t="s">
+        <v>68</v>
+      </c>
+      <c r="X62" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y62" s="1"/>
+    </row>
+    <row r="63" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H63" t="s">
         <v>22</v>
       </c>
@@ -1873,8 +2669,21 @@
         <v>57</v>
       </c>
       <c r="L63" s="1"/>
-    </row>
-    <row r="64" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U63" t="s">
+        <v>23</v>
+      </c>
+      <c r="V63" t="s">
+        <v>66</v>
+      </c>
+      <c r="W63" t="s">
+        <v>69</v>
+      </c>
+      <c r="X63" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y63" s="1"/>
+    </row>
+    <row r="64" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H64" t="s">
         <v>22</v>
       </c>
@@ -1888,8 +2697,21 @@
         <v>57</v>
       </c>
       <c r="L64" s="1"/>
-    </row>
-    <row r="65" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U64" t="s">
+        <v>23</v>
+      </c>
+      <c r="V64" t="s">
+        <v>66</v>
+      </c>
+      <c r="W64" t="s">
+        <v>70</v>
+      </c>
+      <c r="X64" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y64" s="1"/>
+    </row>
+    <row r="65" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H65" t="s">
         <v>22</v>
       </c>
@@ -1903,8 +2725,21 @@
         <v>57</v>
       </c>
       <c r="L65" s="1"/>
-    </row>
-    <row r="66" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U65" t="s">
+        <v>23</v>
+      </c>
+      <c r="V65" t="s">
+        <v>66</v>
+      </c>
+      <c r="W65" t="s">
+        <v>67</v>
+      </c>
+      <c r="X65" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y65" s="1"/>
+    </row>
+    <row r="66" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H66" t="s">
         <v>22</v>
       </c>
@@ -1918,8 +2753,21 @@
         <v>57</v>
       </c>
       <c r="L66" s="1"/>
-    </row>
-    <row r="67" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U66" t="s">
+        <v>23</v>
+      </c>
+      <c r="V66" t="s">
+        <v>66</v>
+      </c>
+      <c r="W66" t="s">
+        <v>90</v>
+      </c>
+      <c r="X66" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y66" s="1"/>
+    </row>
+    <row r="67" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H67" t="s">
         <v>22</v>
       </c>
@@ -1933,8 +2781,21 @@
         <v>57</v>
       </c>
       <c r="L67" s="1"/>
-    </row>
-    <row r="68" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U67" t="s">
+        <v>23</v>
+      </c>
+      <c r="V67" t="s">
+        <v>66</v>
+      </c>
+      <c r="W67" t="s">
+        <v>100</v>
+      </c>
+      <c r="X67" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y67" s="1"/>
+    </row>
+    <row r="68" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H68" t="s">
         <v>22</v>
       </c>
@@ -1948,8 +2809,36 @@
         <v>57</v>
       </c>
       <c r="L68" s="1"/>
-    </row>
-    <row r="70" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U68" t="s">
+        <v>23</v>
+      </c>
+      <c r="V68" t="s">
+        <v>66</v>
+      </c>
+      <c r="W68" t="s">
+        <v>101</v>
+      </c>
+      <c r="X68" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y68" s="1"/>
+    </row>
+    <row r="69" spans="8:25" x14ac:dyDescent="0.25">
+      <c r="U69" t="s">
+        <v>23</v>
+      </c>
+      <c r="V69" t="s">
+        <v>66</v>
+      </c>
+      <c r="W69" t="s">
+        <v>64</v>
+      </c>
+      <c r="X69" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y69" s="1"/>
+    </row>
+    <row r="70" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H70" t="s">
         <v>23</v>
       </c>
@@ -1963,8 +2852,21 @@
         <v>56</v>
       </c>
       <c r="L70" s="1"/>
-    </row>
-    <row r="71" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U70" t="s">
+        <v>23</v>
+      </c>
+      <c r="V70" t="s">
+        <v>66</v>
+      </c>
+      <c r="W70" t="s">
+        <v>94</v>
+      </c>
+      <c r="X70" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y70" s="1"/>
+    </row>
+    <row r="71" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H71" t="s">
         <v>23</v>
       </c>
@@ -1978,8 +2880,21 @@
         <v>56</v>
       </c>
       <c r="L71" s="1"/>
-    </row>
-    <row r="72" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U71" t="s">
+        <v>23</v>
+      </c>
+      <c r="V71" t="s">
+        <v>66</v>
+      </c>
+      <c r="W71" t="s">
+        <v>95</v>
+      </c>
+      <c r="X71" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y71" s="1"/>
+    </row>
+    <row r="72" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H72" t="s">
         <v>23</v>
       </c>
@@ -1993,8 +2908,21 @@
         <v>56</v>
       </c>
       <c r="L72" s="1"/>
-    </row>
-    <row r="73" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U72" t="s">
+        <v>23</v>
+      </c>
+      <c r="V72" t="s">
+        <v>66</v>
+      </c>
+      <c r="W72" t="s">
+        <v>73</v>
+      </c>
+      <c r="X72" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y72" s="1"/>
+    </row>
+    <row r="73" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H73" t="s">
         <v>23</v>
       </c>
@@ -2008,8 +2936,21 @@
         <v>56</v>
       </c>
       <c r="L73" s="1"/>
-    </row>
-    <row r="74" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U73" t="s">
+        <v>23</v>
+      </c>
+      <c r="V73" t="s">
+        <v>66</v>
+      </c>
+      <c r="W73" t="s">
+        <v>88</v>
+      </c>
+      <c r="X73" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y73" s="1"/>
+    </row>
+    <row r="74" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H74" t="s">
         <v>23</v>
       </c>
@@ -2023,8 +2964,21 @@
         <v>56</v>
       </c>
       <c r="L74" s="1"/>
-    </row>
-    <row r="75" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U74" t="s">
+        <v>23</v>
+      </c>
+      <c r="V74" t="s">
+        <v>66</v>
+      </c>
+      <c r="W74" t="s">
+        <v>89</v>
+      </c>
+      <c r="X74" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y74" s="1"/>
+    </row>
+    <row r="75" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H75" t="s">
         <v>23</v>
       </c>
@@ -2038,8 +2992,21 @@
         <v>56</v>
       </c>
       <c r="L75" s="1"/>
-    </row>
-    <row r="76" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U75" t="s">
+        <v>23</v>
+      </c>
+      <c r="V75" t="s">
+        <v>66</v>
+      </c>
+      <c r="W75" t="s">
+        <v>74</v>
+      </c>
+      <c r="X75" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y75" s="1"/>
+    </row>
+    <row r="76" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H76" t="s">
         <v>23</v>
       </c>
@@ -2053,8 +3020,21 @@
         <v>57</v>
       </c>
       <c r="L76" s="1"/>
-    </row>
-    <row r="77" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U76" t="s">
+        <v>23</v>
+      </c>
+      <c r="V76" t="s">
+        <v>66</v>
+      </c>
+      <c r="W76" t="s">
+        <v>86</v>
+      </c>
+      <c r="X76" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y76" s="1"/>
+    </row>
+    <row r="77" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H77" t="s">
         <v>23</v>
       </c>
@@ -2068,8 +3048,21 @@
         <v>57</v>
       </c>
       <c r="L77" s="1"/>
-    </row>
-    <row r="78" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U77" t="s">
+        <v>23</v>
+      </c>
+      <c r="V77" t="s">
+        <v>66</v>
+      </c>
+      <c r="W77" t="s">
+        <v>87</v>
+      </c>
+      <c r="X77" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y77" s="1"/>
+    </row>
+    <row r="78" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H78" t="s">
         <v>23</v>
       </c>
@@ -2083,8 +3076,21 @@
         <v>57</v>
       </c>
       <c r="L78" s="1"/>
-    </row>
-    <row r="79" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U78" t="s">
+        <v>23</v>
+      </c>
+      <c r="V78" t="s">
+        <v>66</v>
+      </c>
+      <c r="W78" t="s">
+        <v>71</v>
+      </c>
+      <c r="X78" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y78" s="1"/>
+    </row>
+    <row r="79" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H79" t="s">
         <v>23</v>
       </c>
@@ -2098,8 +3104,21 @@
         <v>57</v>
       </c>
       <c r="L79" s="1"/>
-    </row>
-    <row r="80" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U79" t="s">
+        <v>23</v>
+      </c>
+      <c r="V79" t="s">
+        <v>66</v>
+      </c>
+      <c r="W79" t="s">
+        <v>92</v>
+      </c>
+      <c r="X79" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y79" s="1"/>
+    </row>
+    <row r="80" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H80" t="s">
         <v>23</v>
       </c>
@@ -2113,8 +3132,21 @@
         <v>57</v>
       </c>
       <c r="L80" s="1"/>
-    </row>
-    <row r="81" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U80" t="s">
+        <v>23</v>
+      </c>
+      <c r="V80" t="s">
+        <v>66</v>
+      </c>
+      <c r="W80" t="s">
+        <v>91</v>
+      </c>
+      <c r="X80" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y80" s="1"/>
+    </row>
+    <row r="81" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H81" t="s">
         <v>23</v>
       </c>
@@ -2128,8 +3160,21 @@
         <v>57</v>
       </c>
       <c r="L81" s="1"/>
-    </row>
-    <row r="83" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="U81" t="s">
+        <v>23</v>
+      </c>
+      <c r="V81" t="s">
+        <v>66</v>
+      </c>
+      <c r="W81" t="s">
+        <v>93</v>
+      </c>
+      <c r="X81" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y81" s="1"/>
+    </row>
+    <row r="83" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H83" t="s">
         <v>25</v>
       </c>
@@ -2144,7 +3189,7 @@
       </c>
       <c r="L83" s="1"/>
     </row>
-    <row r="84" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H84" t="s">
         <v>25</v>
       </c>
@@ -2159,7 +3204,7 @@
       </c>
       <c r="L84" s="1"/>
     </row>
-    <row r="85" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H85" t="s">
         <v>25</v>
       </c>
@@ -2174,7 +3219,7 @@
       </c>
       <c r="L85" s="1"/>
     </row>
-    <row r="86" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H86" t="s">
         <v>25</v>
       </c>
@@ -2189,7 +3234,7 @@
       </c>
       <c r="L86" s="1"/>
     </row>
-    <row r="87" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H87" t="s">
         <v>25</v>
       </c>
@@ -2204,7 +3249,7 @@
       </c>
       <c r="L87" s="1"/>
     </row>
-    <row r="88" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H88" t="s">
         <v>25</v>
       </c>
@@ -2219,7 +3264,7 @@
       </c>
       <c r="L88" s="1"/>
     </row>
-    <row r="89" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H89" t="s">
         <v>25</v>
       </c>
@@ -2234,7 +3279,7 @@
       </c>
       <c r="L89" s="1"/>
     </row>
-    <row r="90" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H90" t="s">
         <v>25</v>
       </c>
@@ -2249,7 +3294,7 @@
       </c>
       <c r="L90" s="1"/>
     </row>
-    <row r="91" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H91" t="s">
         <v>25</v>
       </c>
@@ -2264,7 +3309,7 @@
       </c>
       <c r="L91" s="1"/>
     </row>
-    <row r="92" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H92" t="s">
         <v>25</v>
       </c>
@@ -2279,7 +3324,7 @@
       </c>
       <c r="L92" s="1"/>
     </row>
-    <row r="93" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H93" t="s">
         <v>25</v>
       </c>
@@ -2294,7 +3339,7 @@
       </c>
       <c r="L93" s="1"/>
     </row>
-    <row r="94" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H94" t="s">
         <v>25</v>
       </c>
@@ -2309,7 +3354,7 @@
       </c>
       <c r="L94" s="1"/>
     </row>
-    <row r="96" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="8:25" x14ac:dyDescent="0.25">
       <c r="H96" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
Updated Test Requirements File Week 9
</commit_message>
<xml_diff>
--- a/UnitTestFile/UniTests.xlsx
+++ b/UnitTestFile/UniTests.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBB1132-E87E-4A3E-8B0C-C0111F19DE32}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738D55F8-1705-4E2E-A8B3-997A5FA1EB05}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2953" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="102">
   <si>
     <t>White Rook</t>
   </si>
@@ -660,7 +660,7 @@
   <dimension ref="C1:Y159"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="R1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="AA32" sqref="AA32"/>
+      <selection activeCell="AC12" sqref="AC12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added More Tests for Week 9
Added More Tests Week 9
</commit_message>
<xml_diff>
--- a/UnitTestFile/UniTests.xlsx
+++ b/UnitTestFile/UniTests.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738D55F8-1705-4E2E-A8B3-997A5FA1EB05}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9880BEFA-7201-4D0B-A7DE-296F4FE7B936}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="102">
   <si>
     <t>White Rook</t>
   </si>
@@ -657,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C1:Y159"/>
+  <dimension ref="C1:AA159"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="R1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="AC12" sqref="AC12"/>
+      <selection activeCell="AA1" sqref="AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,7 +681,7 @@
     <col min="25" max="25" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>3</v>
       </c>
@@ -694,8 +694,11 @@
       <c r="U1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>47</v>
       </c>
@@ -709,7 +712,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>58</v>
       </c>
@@ -765,7 +768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>0</v>
       </c>
@@ -813,7 +816,7 @@
       </c>
       <c r="Y5" s="1"/>
     </row>
-    <row r="6" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>0</v>
       </c>
@@ -861,7 +864,7 @@
       </c>
       <c r="Y6" s="1"/>
     </row>
-    <row r="7" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>20</v>
       </c>
@@ -909,7 +912,7 @@
       </c>
       <c r="Y7" s="1"/>
     </row>
-    <row r="8" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>20</v>
       </c>
@@ -957,7 +960,7 @@
       </c>
       <c r="Y8" s="1"/>
     </row>
-    <row r="9" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>21</v>
       </c>
@@ -1005,7 +1008,7 @@
       </c>
       <c r="Y9" s="1"/>
     </row>
-    <row r="10" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>21</v>
       </c>
@@ -1053,7 +1056,7 @@
       </c>
       <c r="Y10" s="1"/>
     </row>
-    <row r="11" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>22</v>
       </c>
@@ -1101,7 +1104,7 @@
       </c>
       <c r="Y11" s="1"/>
     </row>
-    <row r="12" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>23</v>
       </c>
@@ -1149,7 +1152,7 @@
       </c>
       <c r="Y12" s="1"/>
     </row>
-    <row r="13" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>24</v>
       </c>
@@ -1184,7 +1187,7 @@
       </c>
       <c r="S13" s="1"/>
     </row>
-    <row r="14" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>24</v>
       </c>
@@ -1232,7 +1235,7 @@
       </c>
       <c r="Y14" s="1"/>
     </row>
-    <row r="15" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>24</v>
       </c>
@@ -1283,7 +1286,7 @@
       </c>
       <c r="Y15" s="1"/>
     </row>
-    <row r="16" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
fixed the bishop function and added results from tests
fixed the bishop function and added results from tests
</commit_message>
<xml_diff>
--- a/UnitTestFile/UniTests.xlsx
+++ b/UnitTestFile/UniTests.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E202A3-2E86-4FE6-BE54-9F8A02C76989}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102882EC-DC20-4027-9F1C-30804F726EA7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4001" uniqueCount="146">
   <si>
     <t>White Rook</t>
   </si>
@@ -437,6 +437,27 @@
   </si>
   <si>
     <t>Attack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can Move To can't hit more than one enemy </t>
+  </si>
+  <si>
+    <t>Piece</t>
+  </si>
+  <si>
+    <t>Enemy 1</t>
+  </si>
+  <si>
+    <t>enemy 2</t>
+  </si>
+  <si>
+    <t>Desired Location</t>
+  </si>
+  <si>
+    <t>White Bishop [D5]</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -785,10 +806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D2:AP163"/>
+  <dimension ref="D2:AL163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Y10" sqref="Y10"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AM16" sqref="AM16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,9 +833,11 @@
     <col min="26" max="26" width="14.85546875" customWidth="1"/>
     <col min="27" max="27" width="13" customWidth="1"/>
     <col min="28" max="28" width="14.85546875" customWidth="1"/>
+    <col min="32" max="32" width="19.28515625" customWidth="1"/>
+    <col min="35" max="35" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D2" s="3" t="s">
         <v>100</v>
       </c>
@@ -825,7 +848,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="4:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D3" s="5" t="s">
         <v>98</v>
       </c>
@@ -868,12 +891,12 @@
       <c r="AK3" s="5"/>
       <c r="AL3" s="5"/>
     </row>
-    <row r="4" spans="4:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:38" x14ac:dyDescent="0.25">
       <c r="I4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="4:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>3</v>
       </c>
@@ -887,7 +910,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="4:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>45</v>
       </c>
@@ -915,8 +938,11 @@
       <c r="Z6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="AF6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>54</v>
       </c>
@@ -957,8 +983,11 @@
       <c r="Z7" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="8" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="AF7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>0</v>
       </c>
@@ -1007,11 +1036,26 @@
       <c r="AD8" t="s">
         <v>2</v>
       </c>
-      <c r="AL8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="AF8" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>141</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>142</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>143</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>0</v>
       </c>
@@ -1058,8 +1102,26 @@
         <v>1</v>
       </c>
       <c r="AD9" s="3"/>
-    </row>
-    <row r="10" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="AF9" t="s">
+        <v>144</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ9" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>18</v>
       </c>
@@ -1106,32 +1168,8 @@
         <v>1</v>
       </c>
       <c r="AD10" s="4"/>
-      <c r="AI10" t="s">
-        <v>89</v>
-      </c>
-      <c r="AJ10" t="s">
-        <v>115</v>
-      </c>
-      <c r="AK10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AL10" t="s">
-        <v>117</v>
-      </c>
-      <c r="AM10" t="s">
-        <v>95</v>
-      </c>
-      <c r="AN10" t="s">
-        <v>126</v>
-      </c>
-      <c r="AO10" t="s">
-        <v>127</v>
-      </c>
-      <c r="AP10" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="11" spans="4:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>18</v>
       </c>
@@ -1178,32 +1216,8 @@
         <v>1</v>
       </c>
       <c r="AD11" s="3"/>
-      <c r="AI11" t="s">
-        <v>107</v>
-      </c>
-      <c r="AJ11" t="s">
-        <v>87</v>
-      </c>
-      <c r="AK11" t="s">
-        <v>118</v>
-      </c>
-      <c r="AL11" t="s">
-        <v>119</v>
-      </c>
-      <c r="AM11" t="s">
-        <v>94</v>
-      </c>
-      <c r="AN11" t="s">
-        <v>129</v>
-      </c>
-      <c r="AO11" t="s">
-        <v>130</v>
-      </c>
-      <c r="AP11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="4:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>19</v>
       </c>
@@ -1250,32 +1264,8 @@
         <v>1</v>
       </c>
       <c r="AD12" s="3"/>
-      <c r="AI12" t="s">
-        <v>108</v>
-      </c>
-      <c r="AJ12" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK12" t="s">
-        <v>88</v>
-      </c>
-      <c r="AL12" t="s">
-        <v>77</v>
-      </c>
-      <c r="AM12" t="s">
-        <v>93</v>
-      </c>
-      <c r="AN12" t="s">
-        <v>76</v>
-      </c>
-      <c r="AO12" t="s">
-        <v>84</v>
-      </c>
-      <c r="AP12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="13" spans="4:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>19</v>
       </c>
@@ -1322,32 +1312,8 @@
         <v>1</v>
       </c>
       <c r="AD13" s="3"/>
-      <c r="AI13" t="s">
-        <v>109</v>
-      </c>
-      <c r="AJ13" t="s">
-        <v>121</v>
-      </c>
-      <c r="AK13" t="s">
-        <v>79</v>
-      </c>
-      <c r="AL13" t="s">
-        <v>67</v>
-      </c>
-      <c r="AM13" t="s">
-        <v>68</v>
-      </c>
-      <c r="AN13" t="s">
-        <v>69</v>
-      </c>
-      <c r="AO13" t="s">
-        <v>75</v>
-      </c>
-      <c r="AP13" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="14" spans="4:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>20</v>
       </c>
@@ -1394,32 +1360,8 @@
         <v>1</v>
       </c>
       <c r="AD14" s="3"/>
-      <c r="AI14" t="s">
-        <v>97</v>
-      </c>
-      <c r="AJ14" t="s">
-        <v>96</v>
-      </c>
-      <c r="AK14" t="s">
-        <v>86</v>
-      </c>
-      <c r="AL14" t="s">
-        <v>63</v>
-      </c>
-      <c r="AM14" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN14" t="s">
-        <v>64</v>
-      </c>
-      <c r="AO14" t="s">
-        <v>65</v>
-      </c>
-      <c r="AP14" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="4:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>21</v>
       </c>
@@ -1453,32 +1395,8 @@
         <v>0</v>
       </c>
       <c r="AD15" s="3"/>
-      <c r="AI15" t="s">
-        <v>110</v>
-      </c>
-      <c r="AJ15" t="s">
-        <v>122</v>
-      </c>
-      <c r="AK15" t="s">
-        <v>78</v>
-      </c>
-      <c r="AL15" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM15" t="s">
-        <v>71</v>
-      </c>
-      <c r="AN15" t="s">
-        <v>70</v>
-      </c>
-      <c r="AO15" t="s">
-        <v>74</v>
-      </c>
-      <c r="AP15" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="4:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>22</v>
       </c>
@@ -1525,32 +1443,8 @@
         <v>0</v>
       </c>
       <c r="AD16" s="3"/>
-      <c r="AI16" t="s">
-        <v>111</v>
-      </c>
-      <c r="AJ16" t="s">
-        <v>123</v>
-      </c>
-      <c r="AK16" t="s">
-        <v>90</v>
-      </c>
-      <c r="AL16" t="s">
-        <v>80</v>
-      </c>
-      <c r="AM16" t="s">
-        <v>73</v>
-      </c>
-      <c r="AN16" t="s">
-        <v>81</v>
-      </c>
-      <c r="AO16" t="s">
-        <v>82</v>
-      </c>
-      <c r="AP16" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="17" spans="4:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>22</v>
       </c>
@@ -1600,32 +1494,8 @@
         <v>0</v>
       </c>
       <c r="AD17" s="3"/>
-      <c r="AI17" t="s">
-        <v>112</v>
-      </c>
-      <c r="AJ17" t="s">
-        <v>91</v>
-      </c>
-      <c r="AK17" t="s">
-        <v>124</v>
-      </c>
-      <c r="AL17" t="s">
-        <v>125</v>
-      </c>
-      <c r="AM17" t="s">
-        <v>92</v>
-      </c>
-      <c r="AN17" t="s">
-        <v>135</v>
-      </c>
-      <c r="AO17" t="s">
-        <v>136</v>
-      </c>
-      <c r="AP17" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="4:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>22</v>
       </c>
@@ -1660,7 +1530,7 @@
       </c>
       <c r="AD18" s="3"/>
     </row>
-    <row r="19" spans="4:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>22</v>
       </c>
@@ -1707,11 +1577,8 @@
         <v>0</v>
       </c>
       <c r="AD19" s="3"/>
-      <c r="AL19" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="20" spans="4:42" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>22</v>
       </c>
@@ -1746,7 +1613,7 @@
       </c>
       <c r="AD20" s="3"/>
     </row>
-    <row r="21" spans="4:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>22</v>
       </c>
@@ -1768,7 +1635,7 @@
       </c>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="4:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
         <v>22</v>
       </c>
@@ -1803,7 +1670,7 @@
       </c>
       <c r="AD22" s="3"/>
     </row>
-    <row r="23" spans="4:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>22</v>
       </c>
@@ -1838,7 +1705,7 @@
       </c>
       <c r="AD23" s="3"/>
     </row>
-    <row r="24" spans="4:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>23</v>
       </c>
@@ -1873,7 +1740,7 @@
       </c>
       <c r="AD24" s="3"/>
     </row>
-    <row r="25" spans="4:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>23</v>
       </c>
@@ -1894,6 +1761,9 @@
         <v>80</v>
       </c>
       <c r="M25" s="1"/>
+      <c r="S25" t="s">
+        <v>113</v>
+      </c>
       <c r="Z25" t="s">
         <v>50</v>
       </c>
@@ -1908,7 +1778,7 @@
       </c>
       <c r="AD25" s="3"/>
     </row>
-    <row r="26" spans="4:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>40</v>
       </c>
@@ -1943,7 +1813,7 @@
       </c>
       <c r="AD26" s="3"/>
     </row>
-    <row r="27" spans="4:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>40</v>
       </c>
@@ -1951,6 +1821,30 @@
         <v>27</v>
       </c>
       <c r="F27" s="4"/>
+      <c r="P27" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>115</v>
+      </c>
+      <c r="R27" t="s">
+        <v>116</v>
+      </c>
+      <c r="S27" t="s">
+        <v>117</v>
+      </c>
+      <c r="T27" t="s">
+        <v>95</v>
+      </c>
+      <c r="U27" t="s">
+        <v>126</v>
+      </c>
+      <c r="V27" t="s">
+        <v>127</v>
+      </c>
+      <c r="W27" t="s">
+        <v>128</v>
+      </c>
       <c r="Z27" t="s">
         <v>50</v>
       </c>
@@ -1965,7 +1859,7 @@
       </c>
       <c r="AD27" s="3"/>
     </row>
-    <row r="28" spans="4:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
         <v>41</v>
       </c>
@@ -1986,6 +1880,30 @@
         <v>70</v>
       </c>
       <c r="M28" s="1"/>
+      <c r="P28" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>87</v>
+      </c>
+      <c r="R28" t="s">
+        <v>118</v>
+      </c>
+      <c r="S28" t="s">
+        <v>119</v>
+      </c>
+      <c r="T28" t="s">
+        <v>94</v>
+      </c>
+      <c r="U28" t="s">
+        <v>129</v>
+      </c>
+      <c r="V28" t="s">
+        <v>130</v>
+      </c>
+      <c r="W28" t="s">
+        <v>85</v>
+      </c>
       <c r="Z28" t="s">
         <v>50</v>
       </c>
@@ -2000,7 +1918,7 @@
       </c>
       <c r="AD28" s="3"/>
     </row>
-    <row r="29" spans="4:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>41</v>
       </c>
@@ -2021,6 +1939,30 @@
         <v>82</v>
       </c>
       <c r="M29" s="1"/>
+      <c r="P29" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>120</v>
+      </c>
+      <c r="R29" t="s">
+        <v>88</v>
+      </c>
+      <c r="S29" t="s">
+        <v>77</v>
+      </c>
+      <c r="T29" t="s">
+        <v>93</v>
+      </c>
+      <c r="U29" t="s">
+        <v>76</v>
+      </c>
+      <c r="V29" t="s">
+        <v>84</v>
+      </c>
+      <c r="W29" t="s">
+        <v>131</v>
+      </c>
       <c r="Z29" t="s">
         <v>50</v>
       </c>
@@ -2035,7 +1977,7 @@
       </c>
       <c r="AD29" s="3"/>
     </row>
-    <row r="30" spans="4:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>42</v>
       </c>
@@ -2056,6 +1998,30 @@
         <v>83</v>
       </c>
       <c r="M30" s="1"/>
+      <c r="P30" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>121</v>
+      </c>
+      <c r="R30" t="s">
+        <v>79</v>
+      </c>
+      <c r="S30" t="s">
+        <v>67</v>
+      </c>
+      <c r="T30" t="s">
+        <v>68</v>
+      </c>
+      <c r="U30" t="s">
+        <v>69</v>
+      </c>
+      <c r="V30" t="s">
+        <v>75</v>
+      </c>
+      <c r="W30" t="s">
+        <v>132</v>
+      </c>
       <c r="Z30" t="s">
         <v>50</v>
       </c>
@@ -2070,7 +2036,7 @@
       </c>
       <c r="AD30" s="3"/>
     </row>
-    <row r="31" spans="4:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
         <v>43</v>
       </c>
@@ -2091,6 +2057,30 @@
         <v>69</v>
       </c>
       <c r="M31" s="1"/>
+      <c r="P31" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>96</v>
+      </c>
+      <c r="R31" t="s">
+        <v>86</v>
+      </c>
+      <c r="S31" t="s">
+        <v>63</v>
+      </c>
+      <c r="T31" t="s">
+        <v>62</v>
+      </c>
+      <c r="U31" t="s">
+        <v>64</v>
+      </c>
+      <c r="V31" t="s">
+        <v>65</v>
+      </c>
+      <c r="W31" t="s">
+        <v>66</v>
+      </c>
       <c r="Z31" t="s">
         <v>50</v>
       </c>
@@ -2105,7 +2095,7 @@
       </c>
       <c r="AD31" s="3"/>
     </row>
-    <row r="32" spans="4:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
         <v>44</v>
       </c>
@@ -2126,6 +2116,30 @@
         <v>84</v>
       </c>
       <c r="M32" s="1"/>
+      <c r="P32" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>122</v>
+      </c>
+      <c r="R32" t="s">
+        <v>78</v>
+      </c>
+      <c r="S32" t="s">
+        <v>60</v>
+      </c>
+      <c r="T32" t="s">
+        <v>71</v>
+      </c>
+      <c r="U32" t="s">
+        <v>70</v>
+      </c>
+      <c r="V32" t="s">
+        <v>74</v>
+      </c>
+      <c r="W32" t="s">
+        <v>133</v>
+      </c>
       <c r="Z32" t="s">
         <v>50</v>
       </c>
@@ -2161,6 +2175,30 @@
         <v>85</v>
       </c>
       <c r="M33" s="1"/>
+      <c r="P33" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>123</v>
+      </c>
+      <c r="R33" t="s">
+        <v>90</v>
+      </c>
+      <c r="S33" t="s">
+        <v>80</v>
+      </c>
+      <c r="T33" t="s">
+        <v>73</v>
+      </c>
+      <c r="U33" t="s">
+        <v>81</v>
+      </c>
+      <c r="V33" t="s">
+        <v>82</v>
+      </c>
+      <c r="W33" t="s">
+        <v>134</v>
+      </c>
       <c r="Z33" t="s">
         <v>50</v>
       </c>
@@ -2196,6 +2234,30 @@
         <v>67</v>
       </c>
       <c r="M34" s="1"/>
+      <c r="P34" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>91</v>
+      </c>
+      <c r="R34" t="s">
+        <v>124</v>
+      </c>
+      <c r="S34" t="s">
+        <v>125</v>
+      </c>
+      <c r="T34" t="s">
+        <v>92</v>
+      </c>
+      <c r="U34" t="s">
+        <v>135</v>
+      </c>
+      <c r="V34" t="s">
+        <v>136</v>
+      </c>
+      <c r="W34" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="35" spans="4:30" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
@@ -2253,6 +2315,9 @@
         <v>87</v>
       </c>
       <c r="M36" s="1"/>
+      <c r="S36" t="s">
+        <v>114</v>
+      </c>
       <c r="Z36" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
Added All files for unit testing
I added all the files with their required unit tests, Must clean up the format and begin giving the unit tests out to other developers to let them write it up
</commit_message>
<xml_diff>
--- a/UnitTestFile/UniTests.xlsx
+++ b/UnitTestFile/UniTests.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B4A96A-50C7-421F-8FAC-4D5C8C44F6F0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3066DF5A-1F8B-4D32-B968-4FF4EDF458DA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1270" uniqueCount="267">
   <si>
     <t>White Rook</t>
   </si>
@@ -480,6 +480,348 @@
   </si>
   <si>
     <t>Week9(Second Week)</t>
+  </si>
+  <si>
+    <t>Week 10 (Third Week)</t>
+  </si>
+  <si>
+    <t>Play Card Function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in </t>
+  </si>
+  <si>
+    <t>Player(PlayerColour player)</t>
+  </si>
+  <si>
+    <t>Player.cs</t>
+  </si>
+  <si>
+    <t>No Test Required</t>
+  </si>
+  <si>
+    <t>DrawHand()</t>
+  </si>
+  <si>
+    <t>File In</t>
+  </si>
+  <si>
+    <t>Test Required</t>
+  </si>
+  <si>
+    <t>PlayCard()</t>
+  </si>
+  <si>
+    <t>Don’t need to test constructor</t>
+  </si>
+  <si>
+    <t>DoClick</t>
+  </si>
+  <si>
+    <t>LoadResources()</t>
+  </si>
+  <si>
+    <t>HelperFunctions.cs</t>
+  </si>
+  <si>
+    <t>No test Required</t>
+  </si>
+  <si>
+    <t>GetRelativePosition(Position origin, Position end)</t>
+  </si>
+  <si>
+    <t>GetNewPosition(Position position, List&lt;int&gt; deltaPosition)</t>
+  </si>
+  <si>
+    <t>Test the output of the function. Is It Accurate?</t>
+  </si>
+  <si>
+    <t>Position GetNewPosition(Position position, int deltaX, int deltaY)</t>
+  </si>
+  <si>
+    <t>PositionClicked ()</t>
+  </si>
+  <si>
+    <t>Function is based on user input which cannot be unit tested and as a result needs to be QA tested</t>
+  </si>
+  <si>
+    <t>Function is based on user input which cannot be unit tested and as a result need to be QA tested</t>
+  </si>
+  <si>
+    <t>GetAbsPos(Position position)</t>
+  </si>
+  <si>
+    <t>GetOpponent(PlayerColour player)</t>
+  </si>
+  <si>
+    <t>Setup(int position)</t>
+  </si>
+  <si>
+    <t>Reason / Tests to be performed</t>
+  </si>
+  <si>
+    <t>Test to see if the board is setup correctly</t>
+  </si>
+  <si>
+    <t>Test to see if the correct colour is being outputted</t>
+  </si>
+  <si>
+    <t>Game.cs</t>
+  </si>
+  <si>
+    <t>Game()</t>
+  </si>
+  <si>
+    <t>DoMove()</t>
+  </si>
+  <si>
+    <t>Play()</t>
+  </si>
+  <si>
+    <t>Setup()</t>
+  </si>
+  <si>
+    <t>Draw()</t>
+  </si>
+  <si>
+    <t>This uses swingame and cannot be tested</t>
+  </si>
+  <si>
+    <t>This is entirely based on SwinGame and cant be tested.</t>
+  </si>
+  <si>
+    <t>Function is loading resources with SwinGame. No test can be made.</t>
+  </si>
+  <si>
+    <t>This is the setup function and cant be tested as it uses Swingame (GUI)</t>
+  </si>
+  <si>
+    <t>GameMain.cs</t>
+  </si>
+  <si>
+    <t>Untesstable</t>
+  </si>
+  <si>
+    <t>Main()</t>
+  </si>
+  <si>
+    <t>Board.cs</t>
+  </si>
+  <si>
+    <t>Board()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test to see if the baord </t>
+  </si>
+  <si>
+    <t>Add(Position position, Piece piece)</t>
+  </si>
+  <si>
+    <t>Remove(Position position)</t>
+  </si>
+  <si>
+    <t>Test to see if No item there / add item / see if item is there</t>
+  </si>
+  <si>
+    <t>Test setup the board and make sure the peaces are in their squares</t>
+  </si>
+  <si>
+    <t>Test to see if there is a piece in a squre / remove it / see if piece is gone.</t>
+  </si>
+  <si>
+    <t>CurrentBoardState()</t>
+  </si>
+  <si>
+    <t>Requires swingame. Untestable</t>
+  </si>
+  <si>
+    <t>Test the output to see if there are pieces in each square. (add 4 pieces to the board then run this function and confirm they are there)</t>
+  </si>
+  <si>
+    <t>Find(Position position)</t>
+  </si>
+  <si>
+    <t>Find(Kind kind, PlayerColour player)</t>
+  </si>
+  <si>
+    <t>FindList(Kind kind, PlayerColour player)</t>
+  </si>
+  <si>
+    <t>GetPositionLocation(Position position)</t>
+  </si>
+  <si>
+    <t>Contains(Kind kind, PlayerColour player)</t>
+  </si>
+  <si>
+    <t>Draw(Piece selected)</t>
+  </si>
+  <si>
+    <t>IsClear(Position begin, Position end)</t>
+  </si>
+  <si>
+    <t>Count(Kind kind)</t>
+  </si>
+  <si>
+    <t>Count(Kind kind, PlayerColour player)</t>
+  </si>
+  <si>
+    <t>Count(PlayerColour player)</t>
+  </si>
+  <si>
+    <t>Test this by adding a piece to the boardand using this to find its location / confirm output</t>
+  </si>
+  <si>
+    <t>Test this by adding pieces to the board from both black and white player teams and then run this function / confirm the location is correct.</t>
+  </si>
+  <si>
+    <t>Test this by adding 5 black and 5 white pieces of a sort, then run this to output their position / confirm output.</t>
+  </si>
+  <si>
+    <t>Test this by giving the function X and Y cordinates then confirm the output of the function.</t>
+  </si>
+  <si>
+    <t>Test this by giving it a pice kind and a player colour, this would then return at least 1 piece of that kind and the player. Confirm output</t>
+  </si>
+  <si>
+    <t>Function is using swingames. Unable to tesst</t>
+  </si>
+  <si>
+    <t>Input position begin and end and confirm the output (true or false) with expected</t>
+  </si>
+  <si>
+    <t>Test this by  placing 3 white pieces of the same type and 5 black piece of the same type on a board, output should be 8.</t>
+  </si>
+  <si>
+    <t>Test this by placing 3 white picees of the same type and 5 black pieces of the same type on a board, test to see how many white then back there are.</t>
+  </si>
+  <si>
+    <t>Test this by adding a few pices of a colour to the board, ask this to count how many pieces the owner has.</t>
+  </si>
+  <si>
+    <t>Rook.cs</t>
+  </si>
+  <si>
+    <t>Queen.cs</t>
+  </si>
+  <si>
+    <t>CanMoveTo (Board board, Position position)</t>
+  </si>
+  <si>
+    <t>NewPosition (Position position)</t>
+  </si>
+  <si>
+    <t>Test this by setting up a rook and moving it to a board location that’s valid to the rooks movement map</t>
+  </si>
+  <si>
+    <t>This is just a slave function to the CanMoveTo function and doesent require testing</t>
+  </si>
+  <si>
+    <t>CanMoveTo(Board board, Position position)</t>
+  </si>
+  <si>
+    <t>Test this by setting up a Queen and moving it to a board location that’s valid to the Queens movement map</t>
+  </si>
+  <si>
+    <t>Piece.cs</t>
+  </si>
+  <si>
+    <t>NewPosition(Position position)</t>
+  </si>
+  <si>
+    <t>ToString()</t>
+  </si>
+  <si>
+    <t>Draw(Board board)</t>
+  </si>
+  <si>
+    <t>MoveMap(Board board)</t>
+  </si>
+  <si>
+    <t>This just parses the new position to the local variable position</t>
+  </si>
+  <si>
+    <t>Test the output of this function and make sure its accurate</t>
+  </si>
+  <si>
+    <t>This test uses Swingames and user input</t>
+  </si>
+  <si>
+    <t>Pawn.cs</t>
+  </si>
+  <si>
+    <t>Test this by setting up a Pawn and moving it to a board location that’s valid to the Pawn movement map</t>
+  </si>
+  <si>
+    <t>NullPiece.cs</t>
+  </si>
+  <si>
+    <t>Test this by making ssure the piece cant move. (bool)</t>
+  </si>
+  <si>
+    <t>Knight.cs</t>
+  </si>
+  <si>
+    <t>Test this by setting up a Knight and moving it to a board location that’s valid to the Knight's movement map</t>
+  </si>
+  <si>
+    <t>King.cs</t>
+  </si>
+  <si>
+    <t>Test this by setting up a King and moving it to a board location that’s valid to the King's movement map</t>
+  </si>
+  <si>
+    <t>Bishop.cs</t>
+  </si>
+  <si>
+    <t>Test this by setting up a Bishop and moving it to a board location that’s valid to the Bishop movement map</t>
+  </si>
+  <si>
+    <t>Cards.cs</t>
+  </si>
+  <si>
+    <t>DrawSmall(int count)</t>
+  </si>
+  <si>
+    <t>DrawLarge(int x, int y)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> KillPiece(Kind kind, PlayerColour owner, int turn) : base(turn, owner)</t>
+  </si>
+  <si>
+    <t>IsPlayable(Game game)</t>
+  </si>
+  <si>
+    <t>Resolve(Game game)</t>
+  </si>
+  <si>
+    <t>Promote (int turn, PlayerColour owner, List&lt;Kind&gt; targets, List&lt;Kind&gt; promotionOptions) : base(turn, owner)</t>
+  </si>
+  <si>
+    <t>Demote(int turn, PlayerColour owner, List&lt;Kind&gt; targets, List&lt;Kind&gt; promotionOptions) : base(turn, owner)</t>
+  </si>
+  <si>
+    <t>FourHorsemen(int turn, PlayerColour player) : base(turn, player)</t>
+  </si>
+  <si>
+    <t>Castle(int turn, PlayerColour oSidestep(int turn, PlayerColour player) : base(turn, player) { }wner) : base(turn, owner)</t>
+  </si>
+  <si>
+    <t>Matricide(int turn, PlayerColour player) : base(turn, player) { }</t>
+  </si>
+  <si>
+    <t>Swap(int turn, PlayerColour player) : base(turn, player) { }</t>
+  </si>
+  <si>
+    <t>PapalRenunciation(int turn, PlayerColour player) : base(turn, player) { }</t>
+  </si>
+  <si>
+    <t>PapalElection(int turn, PlayerColour player) : base(turn, player) { }</t>
+  </si>
+  <si>
+    <t>This can be tested for EACH of the following cards</t>
+  </si>
+  <si>
+    <t>This can be tested by inputting required information</t>
   </si>
 </sst>
 </file>
@@ -501,7 +843,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -544,6 +886,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -557,23 +905,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -856,8 +1207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AL181"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="J31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P43" sqref="P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,10 +1222,11 @@
     <col min="9" max="9" width="14.5703125" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.5703125" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.5703125" customWidth="1"/>
-    <col min="20" max="20" width="12.28515625" customWidth="1"/>
+    <col min="16" max="16" width="55.5703125" customWidth="1"/>
+    <col min="17" max="17" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11.7109375" customWidth="1"/>
     <col min="22" max="22" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15.7109375" bestFit="1" customWidth="1"/>
@@ -898,45 +1250,47 @@
       </c>
     </row>
     <row r="3" spans="2:38" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="6" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
-      <c r="W3" s="9"/>
-      <c r="AB3" s="5" t="s">
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="6"/>
+      <c r="AB3" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AC3" s="5"/>
-      <c r="AD3" s="5"/>
-      <c r="AE3" s="5"/>
-      <c r="AF3" s="5"/>
-      <c r="AG3" s="5"/>
-      <c r="AH3" s="5"/>
-      <c r="AI3" s="5"/>
-      <c r="AJ3" s="5"/>
-      <c r="AK3" s="5"/>
-      <c r="AL3" s="5"/>
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="7"/>
+      <c r="AE3" s="7"/>
+      <c r="AF3" s="7"/>
+      <c r="AG3" s="7"/>
+      <c r="AH3" s="7"/>
+      <c r="AI3" s="7"/>
+      <c r="AJ3" s="7"/>
+      <c r="AK3" s="7"/>
+      <c r="AL3" s="7"/>
     </row>
     <row r="5" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -953,6 +1307,21 @@
       <c r="I6" t="s">
         <v>55</v>
       </c>
+      <c r="P6" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>155</v>
+      </c>
+      <c r="R6" t="s">
+        <v>160</v>
+      </c>
+      <c r="S6" t="s">
+        <v>161</v>
+      </c>
+      <c r="T6" t="s">
+        <v>178</v>
+      </c>
       <c r="AF6" t="s">
         <v>3</v>
       </c>
@@ -970,6 +1339,21 @@
       <c r="I7" t="s">
         <v>56</v>
       </c>
+      <c r="P7" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>155</v>
+      </c>
+      <c r="R7" t="s">
+        <v>157</v>
+      </c>
+      <c r="S7" t="s">
+        <v>158</v>
+      </c>
+      <c r="T7" t="s">
+        <v>163</v>
+      </c>
       <c r="AF7" t="s">
         <v>135</v>
       </c>
@@ -1003,6 +1387,21 @@
       <c r="M8" t="s">
         <v>2</v>
       </c>
+      <c r="P8" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>155</v>
+      </c>
+      <c r="R8" t="s">
+        <v>157</v>
+      </c>
+      <c r="S8" t="s">
+        <v>158</v>
+      </c>
+      <c r="T8" t="s">
+        <v>174</v>
+      </c>
       <c r="AF8" t="s">
         <v>136</v>
       </c>
@@ -1046,6 +1445,21 @@
         <v>53</v>
       </c>
       <c r="M9" s="3"/>
+      <c r="P9" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>155</v>
+      </c>
+      <c r="R9" t="s">
+        <v>157</v>
+      </c>
+      <c r="S9" t="s">
+        <v>158</v>
+      </c>
+      <c r="T9" t="s">
+        <v>174</v>
+      </c>
       <c r="AF9" t="s">
         <v>140</v>
       </c>
@@ -1089,6 +1503,21 @@
         <v>53</v>
       </c>
       <c r="M10" s="3"/>
+      <c r="P10" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>155</v>
+      </c>
+      <c r="R10" t="s">
+        <v>157</v>
+      </c>
+      <c r="S10" t="s">
+        <v>158</v>
+      </c>
+      <c r="T10" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="11" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -1111,6 +1540,21 @@
         <v>53</v>
       </c>
       <c r="M11" s="3"/>
+      <c r="P11" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>155</v>
+      </c>
+      <c r="R11" t="s">
+        <v>166</v>
+      </c>
+      <c r="S11" t="s">
+        <v>167</v>
+      </c>
+      <c r="T11" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="12" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -1133,6 +1577,21 @@
         <v>53</v>
       </c>
       <c r="M12" s="3"/>
+      <c r="P12" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>155</v>
+      </c>
+      <c r="R12" t="s">
+        <v>166</v>
+      </c>
+      <c r="S12" t="s">
+        <v>161</v>
+      </c>
+      <c r="T12" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="13" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -1155,6 +1614,21 @@
         <v>53</v>
       </c>
       <c r="M13" s="3"/>
+      <c r="P13" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>155</v>
+      </c>
+      <c r="R13" t="s">
+        <v>166</v>
+      </c>
+      <c r="S13" t="s">
+        <v>161</v>
+      </c>
+      <c r="T13" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="14" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -1177,6 +1651,21 @@
         <v>53</v>
       </c>
       <c r="M14" s="3"/>
+      <c r="P14" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>155</v>
+      </c>
+      <c r="R14" t="s">
+        <v>166</v>
+      </c>
+      <c r="S14" t="s">
+        <v>161</v>
+      </c>
+      <c r="T14" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="15" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -1199,6 +1688,21 @@
         <v>53</v>
       </c>
       <c r="M15" s="3"/>
+      <c r="P15" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>155</v>
+      </c>
+      <c r="R15" t="s">
+        <v>166</v>
+      </c>
+      <c r="S15" t="s">
+        <v>158</v>
+      </c>
+      <c r="T15" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="16" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -1221,8 +1725,23 @@
         <v>53</v>
       </c>
       <c r="M16" s="3"/>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P16" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>155</v>
+      </c>
+      <c r="R16" t="s">
+        <v>166</v>
+      </c>
+      <c r="S16" t="s">
+        <v>161</v>
+      </c>
+      <c r="T16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>22</v>
       </c>
@@ -1243,8 +1762,23 @@
         <v>53</v>
       </c>
       <c r="M17" s="3"/>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P17" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>155</v>
+      </c>
+      <c r="R17" t="s">
+        <v>166</v>
+      </c>
+      <c r="S17" t="s">
+        <v>161</v>
+      </c>
+      <c r="T17" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>22</v>
       </c>
@@ -1265,8 +1799,23 @@
         <v>53</v>
       </c>
       <c r="M18" s="3"/>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P18" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>155</v>
+      </c>
+      <c r="R18" t="s">
+        <v>166</v>
+      </c>
+      <c r="S18" t="s">
+        <v>161</v>
+      </c>
+      <c r="T18" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>22</v>
       </c>
@@ -1287,8 +1836,23 @@
         <v>53</v>
       </c>
       <c r="M19" s="3"/>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P19" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>155</v>
+      </c>
+      <c r="R19" t="s">
+        <v>191</v>
+      </c>
+      <c r="S19" t="s">
+        <v>158</v>
+      </c>
+      <c r="T19" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>22</v>
       </c>
@@ -1309,8 +1873,23 @@
         <v>53</v>
       </c>
       <c r="M20" s="3"/>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P20" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>155</v>
+      </c>
+      <c r="R20" t="s">
+        <v>181</v>
+      </c>
+      <c r="S20" t="s">
+        <v>158</v>
+      </c>
+      <c r="T20" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>22</v>
       </c>
@@ -1318,8 +1897,23 @@
         <v>14</v>
       </c>
       <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P21" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>155</v>
+      </c>
+      <c r="R21" t="s">
+        <v>181</v>
+      </c>
+      <c r="S21" t="s">
+        <v>158</v>
+      </c>
+      <c r="T21" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>22</v>
       </c>
@@ -1327,8 +1921,23 @@
         <v>16</v>
       </c>
       <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P22" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>155</v>
+      </c>
+      <c r="R22" t="s">
+        <v>181</v>
+      </c>
+      <c r="S22" t="s">
+        <v>158</v>
+      </c>
+      <c r="T22" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>22</v>
       </c>
@@ -1336,8 +1945,23 @@
         <v>17</v>
       </c>
       <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P23" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>155</v>
+      </c>
+      <c r="R23" t="s">
+        <v>181</v>
+      </c>
+      <c r="S23" t="s">
+        <v>158</v>
+      </c>
+      <c r="T23" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>23</v>
       </c>
@@ -1348,8 +1972,23 @@
       <c r="I24" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P24" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>155</v>
+      </c>
+      <c r="R24" t="s">
+        <v>181</v>
+      </c>
+      <c r="S24" t="s">
+        <v>161</v>
+      </c>
+      <c r="T24" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>23</v>
       </c>
@@ -1360,8 +1999,23 @@
       <c r="I25" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P25" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>155</v>
+      </c>
+      <c r="R25" t="s">
+        <v>181</v>
+      </c>
+      <c r="S25" t="s">
+        <v>158</v>
+      </c>
+      <c r="T25" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>40</v>
       </c>
@@ -1384,8 +2038,23 @@
       <c r="M26" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P26" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>155</v>
+      </c>
+      <c r="R26" t="s">
+        <v>194</v>
+      </c>
+      <c r="S26" t="s">
+        <v>158</v>
+      </c>
+      <c r="T26" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>40</v>
       </c>
@@ -1406,8 +2075,23 @@
         <v>1</v>
       </c>
       <c r="M27" s="3"/>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P27" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>155</v>
+      </c>
+      <c r="R27" t="s">
+        <v>194</v>
+      </c>
+      <c r="S27" t="s">
+        <v>161</v>
+      </c>
+      <c r="T27" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>41</v>
       </c>
@@ -1428,8 +2112,23 @@
         <v>1</v>
       </c>
       <c r="M28" s="4"/>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P28" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>155</v>
+      </c>
+      <c r="R28" t="s">
+        <v>194</v>
+      </c>
+      <c r="S28" t="s">
+        <v>161</v>
+      </c>
+      <c r="T28" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>41</v>
       </c>
@@ -1450,8 +2149,23 @@
         <v>1</v>
       </c>
       <c r="M29" s="3"/>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P29" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>155</v>
+      </c>
+      <c r="R29" t="s">
+        <v>194</v>
+      </c>
+      <c r="S29" t="s">
+        <v>161</v>
+      </c>
+      <c r="T29" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>42</v>
       </c>
@@ -1472,8 +2186,23 @@
         <v>1</v>
       </c>
       <c r="M30" s="3"/>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P30" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>155</v>
+      </c>
+      <c r="R30" t="s">
+        <v>194</v>
+      </c>
+      <c r="S30" t="s">
+        <v>161</v>
+      </c>
+      <c r="T30" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>43</v>
       </c>
@@ -1494,8 +2223,23 @@
         <v>1</v>
       </c>
       <c r="M31" s="3"/>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P31" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>155</v>
+      </c>
+      <c r="R31" t="s">
+        <v>194</v>
+      </c>
+      <c r="S31" t="s">
+        <v>161</v>
+      </c>
+      <c r="T31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>44</v>
       </c>
@@ -1516,8 +2260,23 @@
         <v>1</v>
       </c>
       <c r="M32" s="3"/>
-    </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P32" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>155</v>
+      </c>
+      <c r="R32" t="s">
+        <v>194</v>
+      </c>
+      <c r="S32" t="s">
+        <v>161</v>
+      </c>
+      <c r="T32" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>44</v>
       </c>
@@ -1538,8 +2297,23 @@
         <v>0</v>
       </c>
       <c r="M33" s="3"/>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P33" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>155</v>
+      </c>
+      <c r="R33" t="s">
+        <v>194</v>
+      </c>
+      <c r="S33" t="s">
+        <v>161</v>
+      </c>
+      <c r="T33" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>44</v>
       </c>
@@ -1560,8 +2334,23 @@
         <v>0</v>
       </c>
       <c r="M34" s="3"/>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P34" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>155</v>
+      </c>
+      <c r="R34" t="s">
+        <v>194</v>
+      </c>
+      <c r="S34" t="s">
+        <v>161</v>
+      </c>
+      <c r="T34" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>44</v>
       </c>
@@ -1582,8 +2371,23 @@
         <v>0</v>
       </c>
       <c r="M35" s="3"/>
-    </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P35" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>155</v>
+      </c>
+      <c r="R35" t="s">
+        <v>194</v>
+      </c>
+      <c r="S35" t="s">
+        <v>161</v>
+      </c>
+      <c r="T35" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>44</v>
       </c>
@@ -1604,8 +2408,23 @@
         <v>0</v>
       </c>
       <c r="M36" s="3"/>
-    </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P36" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>155</v>
+      </c>
+      <c r="R36" t="s">
+        <v>194</v>
+      </c>
+      <c r="S36" t="s">
+        <v>158</v>
+      </c>
+      <c r="T36" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>44</v>
       </c>
@@ -1626,8 +2445,23 @@
         <v>0</v>
       </c>
       <c r="M37" s="3"/>
-    </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P37" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>155</v>
+      </c>
+      <c r="R37" t="s">
+        <v>194</v>
+      </c>
+      <c r="S37" t="s">
+        <v>161</v>
+      </c>
+      <c r="T37" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>44</v>
       </c>
@@ -1648,8 +2482,23 @@
         <v>0</v>
       </c>
       <c r="M38" s="3"/>
-    </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P38" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>155</v>
+      </c>
+      <c r="R38" t="s">
+        <v>194</v>
+      </c>
+      <c r="S38" t="s">
+        <v>161</v>
+      </c>
+      <c r="T38" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>44</v>
       </c>
@@ -1657,8 +2506,23 @@
         <v>39</v>
       </c>
       <c r="D39" s="4"/>
-    </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P39" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>155</v>
+      </c>
+      <c r="R39" t="s">
+        <v>194</v>
+      </c>
+      <c r="S39" t="s">
+        <v>161</v>
+      </c>
+      <c r="T39" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
       <c r="I40" t="s">
         <v>50</v>
       </c>
@@ -1672,8 +2536,23 @@
         <v>1</v>
       </c>
       <c r="M40" s="3"/>
-    </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P40" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>155</v>
+      </c>
+      <c r="R40" t="s">
+        <v>194</v>
+      </c>
+      <c r="S40" t="s">
+        <v>161</v>
+      </c>
+      <c r="T40" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
       <c r="I41" t="s">
         <v>50</v>
       </c>
@@ -1687,8 +2566,23 @@
         <v>1</v>
       </c>
       <c r="M41" s="3"/>
-    </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P41" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>155</v>
+      </c>
+      <c r="R41" t="s">
+        <v>225</v>
+      </c>
+      <c r="S41" t="s">
+        <v>161</v>
+      </c>
+      <c r="T41" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
       <c r="I42" t="s">
         <v>50</v>
       </c>
@@ -1702,8 +2596,23 @@
         <v>1</v>
       </c>
       <c r="M42" s="3"/>
-    </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P42" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>155</v>
+      </c>
+      <c r="R42" t="s">
+        <v>225</v>
+      </c>
+      <c r="S42" t="s">
+        <v>158</v>
+      </c>
+      <c r="T42" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
       <c r="I43" t="s">
         <v>50</v>
       </c>
@@ -1717,8 +2626,23 @@
         <v>1</v>
       </c>
       <c r="M43" s="3"/>
-    </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P43" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>155</v>
+      </c>
+      <c r="R43" t="s">
+        <v>226</v>
+      </c>
+      <c r="S43" t="s">
+        <v>161</v>
+      </c>
+      <c r="T43" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
       <c r="I44" t="s">
         <v>50</v>
       </c>
@@ -1732,8 +2656,23 @@
         <v>1</v>
       </c>
       <c r="M44" s="3"/>
-    </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P44" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>155</v>
+      </c>
+      <c r="R44" t="s">
+        <v>233</v>
+      </c>
+      <c r="S44" t="s">
+        <v>158</v>
+      </c>
+      <c r="T44" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>61</v>
       </c>
@@ -1756,8 +2695,23 @@
         <v>1</v>
       </c>
       <c r="M45" s="3"/>
-    </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P45" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>155</v>
+      </c>
+      <c r="R45" t="s">
+        <v>233</v>
+      </c>
+      <c r="S45" t="s">
+        <v>161</v>
+      </c>
+      <c r="T45" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>57</v>
       </c>
@@ -1786,8 +2740,23 @@
         <v>0</v>
       </c>
       <c r="M46" s="3"/>
-    </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P46" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>155</v>
+      </c>
+      <c r="R46" t="s">
+        <v>233</v>
+      </c>
+      <c r="S46" t="s">
+        <v>158</v>
+      </c>
+      <c r="T46" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="47" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>20</v>
       </c>
@@ -1814,8 +2783,23 @@
         <v>0</v>
       </c>
       <c r="M47" s="3"/>
-    </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P47" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>155</v>
+      </c>
+      <c r="R47" t="s">
+        <v>233</v>
+      </c>
+      <c r="S47" t="s">
+        <v>158</v>
+      </c>
+      <c r="T47" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="48" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>20</v>
       </c>
@@ -1842,8 +2826,23 @@
         <v>0</v>
       </c>
       <c r="M48" s="3"/>
-    </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P48" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>155</v>
+      </c>
+      <c r="R48" t="s">
+        <v>241</v>
+      </c>
+      <c r="S48" t="s">
+        <v>161</v>
+      </c>
+      <c r="T48" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="49" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>20</v>
       </c>
@@ -1870,8 +2869,23 @@
         <v>0</v>
       </c>
       <c r="M49" s="3"/>
-    </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P49" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>155</v>
+      </c>
+      <c r="R49" t="s">
+        <v>241</v>
+      </c>
+      <c r="S49" t="s">
+        <v>158</v>
+      </c>
+      <c r="T49" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="50" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>20</v>
       </c>
@@ -1898,8 +2912,23 @@
         <v>0</v>
       </c>
       <c r="M50" s="3"/>
-    </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P50" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>155</v>
+      </c>
+      <c r="R50" t="s">
+        <v>243</v>
+      </c>
+      <c r="S50" t="s">
+        <v>161</v>
+      </c>
+      <c r="T50" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="51" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>20</v>
       </c>
@@ -1926,8 +2955,23 @@
         <v>0</v>
       </c>
       <c r="M51" s="3"/>
-    </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P51" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>155</v>
+      </c>
+      <c r="R51" t="s">
+        <v>245</v>
+      </c>
+      <c r="S51" t="s">
+        <v>161</v>
+      </c>
+      <c r="T51" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="52" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>20</v>
       </c>
@@ -1941,8 +2985,23 @@
         <v>64</v>
       </c>
       <c r="F52" s="1"/>
-    </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P52" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>155</v>
+      </c>
+      <c r="R52" t="s">
+        <v>247</v>
+      </c>
+      <c r="S52" t="s">
+        <v>161</v>
+      </c>
+      <c r="T52" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="53" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>20</v>
       </c>
@@ -1969,8 +3028,23 @@
         <v>1</v>
       </c>
       <c r="M53" s="3"/>
-    </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P53" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>155</v>
+      </c>
+      <c r="R53" t="s">
+        <v>247</v>
+      </c>
+      <c r="S53" t="s">
+        <v>158</v>
+      </c>
+      <c r="T53" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="54" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>20</v>
       </c>
@@ -1997,8 +3071,23 @@
         <v>1</v>
       </c>
       <c r="M54" s="3"/>
-    </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P54" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>155</v>
+      </c>
+      <c r="R54" t="s">
+        <v>249</v>
+      </c>
+      <c r="S54" t="s">
+        <v>161</v>
+      </c>
+      <c r="T54" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="55" spans="2:20" x14ac:dyDescent="0.25">
       <c r="I55" t="s">
         <v>51</v>
       </c>
@@ -2012,8 +3101,23 @@
         <v>1</v>
       </c>
       <c r="M55" s="3"/>
-    </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P55" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>155</v>
+      </c>
+      <c r="R55" t="s">
+        <v>251</v>
+      </c>
+      <c r="S55" t="s">
+        <v>158</v>
+      </c>
+      <c r="T55" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="56" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>22</v>
       </c>
@@ -2040,8 +3144,23 @@
         <v>1</v>
       </c>
       <c r="M56" s="3"/>
-    </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P56" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>155</v>
+      </c>
+      <c r="R56" t="s">
+        <v>251</v>
+      </c>
+      <c r="S56" t="s">
+        <v>158</v>
+      </c>
+      <c r="T56" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="57" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>147</v>
       </c>
@@ -2068,8 +3187,23 @@
         <v>1</v>
       </c>
       <c r="M57" s="3"/>
-    </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P57" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>155</v>
+      </c>
+      <c r="R57" t="s">
+        <v>251</v>
+      </c>
+      <c r="S57" t="s">
+        <v>158</v>
+      </c>
+      <c r="T57" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="58" spans="2:20" x14ac:dyDescent="0.25">
       <c r="I58" t="s">
         <v>51</v>
       </c>
@@ -2083,8 +3217,23 @@
         <v>1</v>
       </c>
       <c r="M58" s="3"/>
-    </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P58" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>155</v>
+      </c>
+      <c r="R58" t="s">
+        <v>251</v>
+      </c>
+      <c r="S58" t="s">
+        <v>161</v>
+      </c>
+      <c r="T58" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="59" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>18</v>
       </c>
@@ -2111,8 +3260,23 @@
         <v>0</v>
       </c>
       <c r="M59" s="3"/>
-    </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P59" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>155</v>
+      </c>
+      <c r="R59" t="s">
+        <v>251</v>
+      </c>
+      <c r="S59" t="s">
+        <v>161</v>
+      </c>
+      <c r="T59" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="60" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>18</v>
       </c>
@@ -2139,8 +3303,23 @@
         <v>0</v>
       </c>
       <c r="M60" s="3"/>
-    </row>
-    <row r="61" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P60" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>155</v>
+      </c>
+      <c r="R60" t="s">
+        <v>251</v>
+      </c>
+      <c r="S60" t="s">
+        <v>161</v>
+      </c>
+      <c r="T60" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="61" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>18</v>
       </c>
@@ -2167,8 +3346,23 @@
         <v>0</v>
       </c>
       <c r="M61" s="3"/>
-    </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P61" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>155</v>
+      </c>
+      <c r="R61" t="s">
+        <v>251</v>
+      </c>
+      <c r="S61" t="s">
+        <v>161</v>
+      </c>
+      <c r="T61" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="62" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>18</v>
       </c>
@@ -2195,8 +3389,23 @@
         <v>0</v>
       </c>
       <c r="M62" s="3"/>
-    </row>
-    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P62" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>155</v>
+      </c>
+      <c r="R62" t="s">
+        <v>251</v>
+      </c>
+      <c r="S62" t="s">
+        <v>161</v>
+      </c>
+      <c r="T62" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="63" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>18</v>
       </c>
@@ -2223,8 +3432,23 @@
         <v>0</v>
       </c>
       <c r="M63" s="3"/>
-    </row>
-    <row r="64" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P63" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>155</v>
+      </c>
+      <c r="R63" t="s">
+        <v>251</v>
+      </c>
+      <c r="S63" t="s">
+        <v>161</v>
+      </c>
+      <c r="T63" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="64" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>18</v>
       </c>
@@ -2251,8 +3475,23 @@
         <v>0</v>
       </c>
       <c r="M64" s="3"/>
-    </row>
-    <row r="65" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P64" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>155</v>
+      </c>
+      <c r="R64" t="s">
+        <v>251</v>
+      </c>
+      <c r="S64" t="s">
+        <v>161</v>
+      </c>
+      <c r="T64" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="65" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>18</v>
       </c>
@@ -2266,8 +3505,23 @@
         <v>79</v>
       </c>
       <c r="F65" s="1"/>
-    </row>
-    <row r="66" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P65" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>155</v>
+      </c>
+      <c r="R65" t="s">
+        <v>251</v>
+      </c>
+      <c r="S65" t="s">
+        <v>161</v>
+      </c>
+      <c r="T65" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="66" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>18</v>
       </c>
@@ -2294,8 +3548,23 @@
         <v>1</v>
       </c>
       <c r="M66" s="3"/>
-    </row>
-    <row r="67" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P66" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>155</v>
+      </c>
+      <c r="R66" t="s">
+        <v>251</v>
+      </c>
+      <c r="S66" t="s">
+        <v>161</v>
+      </c>
+      <c r="T66" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="67" spans="2:20" x14ac:dyDescent="0.25">
       <c r="I67" t="s">
         <v>19</v>
       </c>
@@ -2309,8 +3578,23 @@
         <v>1</v>
       </c>
       <c r="M67" s="3"/>
-    </row>
-    <row r="68" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P67" t="s">
+        <v>264</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>155</v>
+      </c>
+      <c r="R67" t="s">
+        <v>251</v>
+      </c>
+      <c r="S67" t="s">
+        <v>161</v>
+      </c>
+      <c r="T67" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="68" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>19</v>
       </c>
@@ -2338,7 +3622,7 @@
       </c>
       <c r="M68" s="3"/>
     </row>
-    <row r="69" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>19</v>
       </c>
@@ -2366,7 +3650,7 @@
       </c>
       <c r="M69" s="3"/>
     </row>
-    <row r="70" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>19</v>
       </c>
@@ -2394,7 +3678,7 @@
       </c>
       <c r="M70" s="3"/>
     </row>
-    <row r="71" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>19</v>
       </c>
@@ -2422,7 +3706,7 @@
       </c>
       <c r="M71" s="3"/>
     </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>19</v>
       </c>
@@ -2450,7 +3734,7 @@
       </c>
       <c r="M72" s="3"/>
     </row>
-    <row r="73" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>19</v>
       </c>
@@ -2478,7 +3762,7 @@
       </c>
       <c r="M73" s="3"/>
     </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>19</v>
       </c>
@@ -2506,7 +3790,7 @@
       </c>
       <c r="M74" s="3"/>
     </row>
-    <row r="75" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>19</v>
       </c>
@@ -2534,7 +3818,7 @@
       </c>
       <c r="M75" s="3"/>
     </row>
-    <row r="76" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>19</v>
       </c>
@@ -2562,7 +3846,7 @@
       </c>
       <c r="M76" s="3"/>
     </row>
-    <row r="77" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>19</v>
       </c>
@@ -2590,7 +3874,7 @@
       </c>
       <c r="M77" s="3"/>
     </row>
-    <row r="78" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>19</v>
       </c>
@@ -2605,7 +3889,7 @@
       </c>
       <c r="F78" s="1"/>
     </row>
-    <row r="79" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>19</v>
       </c>
@@ -2633,7 +3917,7 @@
       </c>
       <c r="M79" s="3"/>
     </row>
-    <row r="80" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>19</v>
       </c>
@@ -3894,7 +5178,7 @@
       <c r="B129" t="b">
         <v>1</v>
       </c>
-      <c r="C129" s="8" t="b">
+      <c r="C129" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I129" t="s">
@@ -3975,7 +5259,7 @@
       <c r="B134" t="b">
         <v>1</v>
       </c>
-      <c r="C134" s="8" t="b">
+      <c r="C134" s="5" t="b">
         <v>1</v>
       </c>
       <c r="I134" t="s">
@@ -4653,10 +5937,11 @@
       <c r="M181" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="AB3:AL3"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="I3:O3"/>
+    <mergeCell ref="P3:V3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Modified Some functionalist tests and unit tets
</commit_message>
<xml_diff>
--- a/UnitTestFile/UniTests.xlsx
+++ b/UnitTestFile/UniTests.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8EB515-4DDF-4A75-8ADD-ACC1A30DB75D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4BFD30-CA63-4D91-8CA9-F191355C8E02}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -886,7 +886,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -935,6 +935,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -948,7 +954,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -971,6 +977,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1253,13 +1260,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AU180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G9" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="37.140625" customWidth="1"/>
+    <col min="2" max="2" width="59.85546875" customWidth="1"/>
     <col min="3" max="3" width="2.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
@@ -1378,8 +1385,8 @@
       </c>
     </row>
     <row r="7" spans="2:47" x14ac:dyDescent="0.25">
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
       <c r="I7" t="s">
         <v>269</v>
       </c>

</xml_diff>

<commit_message>
Piece and Helper Function Unit Tests
</commit_message>
<xml_diff>
--- a/UnitTestFile/UniTests.xlsx
+++ b/UnitTestFile/UniTests.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4BFD30-CA63-4D91-8CA9-F191355C8E02}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07B8178-E25E-4DC5-B2F7-3BE065E0D99E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="283">
   <si>
     <t>White Rook</t>
   </si>
@@ -821,9 +821,6 @@
     <t>0,0</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Pass / Fail - Commends</t>
   </si>
   <si>
@@ -858,6 +855,21 @@
   </si>
   <si>
     <t>Test 2</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>X&amp;Y coordinates</t>
+  </si>
+  <si>
+    <t>PlayerColor.Black</t>
+  </si>
+  <si>
+    <t>B1: Pawn White</t>
+  </si>
+  <si>
+    <t>Board, Position</t>
   </si>
 </sst>
 </file>
@@ -954,7 +966,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -971,13 +983,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1260,46 +1273,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AU180"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J56" sqref="J56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="59.85546875" customWidth="1"/>
-    <col min="3" max="3" width="2.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.88671875" customWidth="1"/>
+    <col min="3" max="3" width="2.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.88671875" customWidth="1"/>
+    <col min="7" max="7" width="25.33203125" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="144" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" customWidth="1"/>
-    <col min="16" max="16" width="19.42578125" customWidth="1"/>
-    <col min="17" max="17" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.28515625" customWidth="1"/>
+    <col min="15" max="15" width="10.88671875" customWidth="1"/>
+    <col min="16" max="16" width="19.44140625" customWidth="1"/>
+    <col min="17" max="17" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.33203125" customWidth="1"/>
     <col min="24" max="24" width="11" customWidth="1"/>
-    <col min="25" max="25" width="15.85546875" customWidth="1"/>
-    <col min="26" max="26" width="17.140625" customWidth="1"/>
+    <col min="25" max="25" width="15.88671875" customWidth="1"/>
+    <col min="26" max="26" width="17.109375" customWidth="1"/>
     <col min="27" max="27" width="13" customWidth="1"/>
-    <col min="28" max="28" width="14.85546875" customWidth="1"/>
-    <col min="29" max="29" width="18.42578125" customWidth="1"/>
-    <col min="32" max="32" width="19.28515625" customWidth="1"/>
-    <col min="35" max="35" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.88671875" customWidth="1"/>
+    <col min="29" max="29" width="18.44140625" customWidth="1"/>
+    <col min="32" max="32" width="19.33203125" customWidth="1"/>
+    <col min="35" max="35" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="14" customWidth="1"/>
-    <col min="49" max="49" width="19.42578125" customWidth="1"/>
-    <col min="55" max="55" width="13.7109375" customWidth="1"/>
-    <col min="57" max="57" width="14.28515625" customWidth="1"/>
+    <col min="49" max="49" width="19.44140625" customWidth="1"/>
+    <col min="55" max="55" width="13.6640625" customWidth="1"/>
+    <col min="57" max="57" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:47" x14ac:dyDescent="0.3">
       <c r="AF2" s="11"/>
       <c r="AG2" s="11"/>
       <c r="AH2" s="11"/>
@@ -1307,44 +1320,44 @@
       <c r="AJ2" s="11"/>
       <c r="AK2" s="11"/>
     </row>
-    <row r="3" spans="2:47" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
+    <row r="3" spans="2:47" x14ac:dyDescent="0.3">
+      <c r="B3" s="14" t="s">
         <v>261</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
-      <c r="O3" s="12" t="s">
+      <c r="O3" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="12"/>
-      <c r="V3" s="12"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="12"/>
-      <c r="Y3" s="12"/>
-      <c r="Z3" s="12"/>
-      <c r="AA3" s="12"/>
-      <c r="AB3" s="12"/>
-      <c r="AC3" s="12"/>
-      <c r="AD3" s="12"/>
-      <c r="AE3" s="12"/>
-      <c r="AF3" s="12"/>
-      <c r="AG3" s="12"/>
-      <c r="AH3" s="12"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
+      <c r="V3" s="13"/>
+      <c r="W3" s="13"/>
+      <c r="X3" s="13"/>
+      <c r="Y3" s="13"/>
+      <c r="Z3" s="13"/>
+      <c r="AA3" s="13"/>
+      <c r="AB3" s="13"/>
+      <c r="AC3" s="13"/>
+      <c r="AD3" s="13"/>
+      <c r="AE3" s="13"/>
+      <c r="AF3" s="13"/>
+      <c r="AG3" s="13"/>
+      <c r="AH3" s="13"/>
       <c r="AI3" s="10"/>
       <c r="AJ3" s="10"/>
       <c r="AK3" s="7"/>
@@ -1359,7 +1372,7 @@
       <c r="AT3" s="7"/>
       <c r="AU3" s="7"/>
     </row>
-    <row r="4" spans="2:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:47" x14ac:dyDescent="0.3">
       <c r="H4" s="3" t="s">
         <v>97</v>
       </c>
@@ -1376,7 +1389,7 @@
       <c r="AJ4" s="11"/>
       <c r="AK4" s="11"/>
     </row>
-    <row r="6" spans="2:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:47" x14ac:dyDescent="0.3">
       <c r="P6" t="s">
         <v>3</v>
       </c>
@@ -1384,11 +1397,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:47" x14ac:dyDescent="0.25">
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
+    <row r="7" spans="2:47" x14ac:dyDescent="0.3">
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
       <c r="I7" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>262</v>
@@ -1397,7 +1410,7 @@
         <v>45</v>
       </c>
       <c r="R7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="W7" t="s">
         <v>55</v>
@@ -1406,13 +1419,13 @@
         <v>134</v>
       </c>
       <c r="AH7" t="s">
+        <v>276</v>
+      </c>
+      <c r="AI7" t="s">
         <v>277</v>
       </c>
-      <c r="AI7" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="8" spans="2:47" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="2:47" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>147</v>
       </c>
@@ -1426,7 +1439,7 @@
         <v>153</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G8" t="s">
         <v>1</v>
@@ -1438,7 +1451,7 @@
         <v>263</v>
       </c>
       <c r="J8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K8" t="s">
         <v>170</v>
@@ -1477,7 +1490,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:47" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>148</v>
       </c>
@@ -1550,7 +1563,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="2:47" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:47" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>151</v>
       </c>
@@ -1600,7 +1613,7 @@
       </c>
       <c r="AA10" s="4"/>
     </row>
-    <row r="11" spans="2:47" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:47" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>154</v>
       </c>
@@ -1650,7 +1663,7 @@
       </c>
       <c r="AA11" s="4"/>
     </row>
-    <row r="12" spans="2:47" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:47" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>156</v>
       </c>
@@ -1700,7 +1713,7 @@
       </c>
       <c r="AA12" s="4"/>
     </row>
-    <row r="13" spans="2:47" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:47" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>157</v>
       </c>
@@ -1750,7 +1763,7 @@
       </c>
       <c r="AA13" s="4"/>
     </row>
-    <row r="14" spans="2:47" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:47" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>160</v>
       </c>
@@ -1764,12 +1777,18 @@
         <v>153</v>
       </c>
       <c r="F14" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="G14" t="s">
         <v>270</v>
       </c>
-      <c r="G14" t="s">
-        <v>271</v>
-      </c>
-      <c r="J14" s="9"/>
+      <c r="H14" t="s">
+        <v>279</v>
+      </c>
+      <c r="I14" t="s">
+        <v>278</v>
+      </c>
+      <c r="J14" s="15"/>
       <c r="K14" t="s">
         <v>162</v>
       </c>
@@ -1794,7 +1813,7 @@
       </c>
       <c r="AA14" s="4"/>
     </row>
-    <row r="15" spans="2:47" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:47" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>161</v>
       </c>
@@ -1808,15 +1827,18 @@
         <v>153</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G15" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H15" t="s">
-        <v>260</v>
-      </c>
-      <c r="J15" s="9"/>
+        <v>90</v>
+      </c>
+      <c r="I15" t="s">
+        <v>278</v>
+      </c>
+      <c r="J15" s="15"/>
       <c r="K15" t="s">
         <v>162</v>
       </c>
@@ -1841,7 +1863,7 @@
       </c>
       <c r="AA15" s="4"/>
     </row>
-    <row r="16" spans="2:47" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:47" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>163</v>
       </c>
@@ -1855,13 +1877,16 @@
         <v>153</v>
       </c>
       <c r="F16" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="G16" t="s">
         <v>273</v>
       </c>
-      <c r="G16" t="s">
-        <v>274</v>
-      </c>
       <c r="H16" t="s">
-        <v>260</v>
+        <v>259</v>
+      </c>
+      <c r="I16" t="s">
+        <v>259</v>
       </c>
       <c r="J16" s="9"/>
       <c r="K16" t="s">
@@ -1888,7 +1913,7 @@
       </c>
       <c r="AA16" s="4"/>
     </row>
-    <row r="17" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>164</v>
       </c>
@@ -1938,7 +1963,7 @@
       </c>
       <c r="AA17" s="4"/>
     </row>
-    <row r="18" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>167</v>
       </c>
@@ -1958,9 +1983,12 @@
         <v>265</v>
       </c>
       <c r="H18" t="s">
-        <v>266</v>
-      </c>
-      <c r="J18" s="3"/>
+        <v>265</v>
+      </c>
+      <c r="I18" t="s">
+        <v>278</v>
+      </c>
+      <c r="J18" s="4"/>
       <c r="K18" t="s">
         <v>162</v>
       </c>
@@ -1985,7 +2013,7 @@
       </c>
       <c r="AA18" s="4"/>
     </row>
-    <row r="19" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>168</v>
       </c>
@@ -2002,12 +2030,15 @@
         <v>109</v>
       </c>
       <c r="G19" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H19" t="s">
-        <v>260</v>
-      </c>
-      <c r="J19" s="3"/>
+        <v>280</v>
+      </c>
+      <c r="I19" t="s">
+        <v>278</v>
+      </c>
+      <c r="J19" s="4"/>
       <c r="K19" t="s">
         <v>172</v>
       </c>
@@ -2032,7 +2063,7 @@
       </c>
       <c r="AA19" s="4"/>
     </row>
-    <row r="20" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>169</v>
       </c>
@@ -2049,12 +2080,15 @@
         <v>106</v>
       </c>
       <c r="G20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H20" t="s">
-        <v>260</v>
-      </c>
-      <c r="J20" s="3"/>
+        <v>281</v>
+      </c>
+      <c r="I20" t="s">
+        <v>278</v>
+      </c>
+      <c r="J20" s="4"/>
       <c r="K20" t="s">
         <v>171</v>
       </c>
@@ -2079,7 +2113,7 @@
       </c>
       <c r="AA20" s="4"/>
     </row>
-    <row r="21" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>185</v>
       </c>
@@ -2129,7 +2163,7 @@
       </c>
       <c r="AA21" s="4"/>
     </row>
-    <row r="22" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>174</v>
       </c>
@@ -2166,7 +2200,7 @@
       </c>
       <c r="R22" s="4"/>
     </row>
-    <row r="23" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>175</v>
       </c>
@@ -2206,7 +2240,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>176</v>
       </c>
@@ -2246,7 +2280,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>154</v>
       </c>
@@ -2298,7 +2332,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>177</v>
       </c>
@@ -2345,7 +2379,7 @@
       </c>
       <c r="AA26" s="4"/>
     </row>
-    <row r="27" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>178</v>
       </c>
@@ -2395,7 +2429,7 @@
       </c>
       <c r="AA27" s="4"/>
     </row>
-    <row r="28" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>187</v>
       </c>
@@ -2445,7 +2479,7 @@
       </c>
       <c r="AA28" s="4"/>
     </row>
-    <row r="29" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>177</v>
       </c>
@@ -2486,7 +2520,7 @@
       </c>
       <c r="AA29" s="4"/>
     </row>
-    <row r="30" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>189</v>
       </c>
@@ -2533,7 +2567,7 @@
       </c>
       <c r="AA30" s="4"/>
     </row>
-    <row r="31" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>190</v>
       </c>
@@ -2580,7 +2614,7 @@
       </c>
       <c r="AA31" s="4"/>
     </row>
-    <row r="32" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>194</v>
       </c>
@@ -2627,7 +2661,7 @@
       </c>
       <c r="AA32" s="4"/>
     </row>
-    <row r="33" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>197</v>
       </c>
@@ -2674,7 +2708,7 @@
       </c>
       <c r="AA33" s="4"/>
     </row>
-    <row r="34" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>198</v>
       </c>
@@ -2721,7 +2755,7 @@
       </c>
       <c r="AA34" s="4"/>
     </row>
-    <row r="35" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>199</v>
       </c>
@@ -2768,7 +2802,7 @@
       </c>
       <c r="AA35" s="4"/>
     </row>
-    <row r="36" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>200</v>
       </c>
@@ -2815,7 +2849,7 @@
       </c>
       <c r="AA36" s="4"/>
     </row>
-    <row r="37" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>201</v>
       </c>
@@ -2862,7 +2896,7 @@
       </c>
       <c r="AA37" s="4"/>
     </row>
-    <row r="38" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>202</v>
       </c>
@@ -2899,7 +2933,7 @@
       </c>
       <c r="R38" s="4"/>
     </row>
-    <row r="39" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>203</v>
       </c>
@@ -2946,7 +2980,7 @@
       </c>
       <c r="AA39" s="4"/>
     </row>
-    <row r="40" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>204</v>
       </c>
@@ -2993,7 +3027,7 @@
       </c>
       <c r="AA40" s="4"/>
     </row>
-    <row r="41" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>205</v>
       </c>
@@ -3033,7 +3067,7 @@
       </c>
       <c r="AA41" s="4"/>
     </row>
-    <row r="42" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>206</v>
       </c>
@@ -3073,7 +3107,7 @@
       </c>
       <c r="AA42" s="4"/>
     </row>
-    <row r="43" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>219</v>
       </c>
@@ -3087,15 +3121,18 @@
         <v>153</v>
       </c>
       <c r="F43" t="s">
-        <v>260</v>
-      </c>
-      <c r="G43" t="s">
-        <v>260</v>
-      </c>
-      <c r="H43" t="s">
-        <v>260</v>
-      </c>
-      <c r="J43" s="3"/>
+        <v>282</v>
+      </c>
+      <c r="G43" t="b">
+        <v>0</v>
+      </c>
+      <c r="H43" t="b">
+        <v>0</v>
+      </c>
+      <c r="I43" t="s">
+        <v>278</v>
+      </c>
+      <c r="J43" s="4"/>
       <c r="K43" t="s">
         <v>221</v>
       </c>
@@ -3113,7 +3150,7 @@
       </c>
       <c r="AA43" s="4"/>
     </row>
-    <row r="44" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>220</v>
       </c>
@@ -3156,7 +3193,7 @@
       </c>
       <c r="AA44" s="4"/>
     </row>
-    <row r="45" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>223</v>
       </c>
@@ -3170,15 +3207,18 @@
         <v>153</v>
       </c>
       <c r="F45" t="s">
-        <v>260</v>
-      </c>
-      <c r="G45" t="s">
-        <v>260</v>
-      </c>
-      <c r="H45" t="s">
-        <v>260</v>
-      </c>
-      <c r="J45" s="3"/>
+        <v>282</v>
+      </c>
+      <c r="G45" t="b">
+        <v>0</v>
+      </c>
+      <c r="H45" t="b">
+        <v>0</v>
+      </c>
+      <c r="I45" t="s">
+        <v>278</v>
+      </c>
+      <c r="J45" s="4"/>
       <c r="K45" t="s">
         <v>224</v>
       </c>
@@ -3196,7 +3236,7 @@
       </c>
       <c r="AA45" s="4"/>
     </row>
-    <row r="46" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>226</v>
       </c>
@@ -3242,7 +3282,7 @@
       </c>
       <c r="AA46" s="4"/>
     </row>
-    <row r="47" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>227</v>
       </c>
@@ -3256,15 +3296,18 @@
         <v>153</v>
       </c>
       <c r="F47" t="s">
-        <v>260</v>
+        <v>107</v>
       </c>
       <c r="G47" t="s">
-        <v>260</v>
+        <v>5</v>
       </c>
       <c r="H47" t="s">
-        <v>260</v>
-      </c>
-      <c r="J47" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="I47" t="s">
+        <v>278</v>
+      </c>
+      <c r="J47" s="4"/>
       <c r="K47" t="s">
         <v>231</v>
       </c>
@@ -3297,7 +3340,7 @@
       </c>
       <c r="AA47" s="4"/>
     </row>
-    <row r="48" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>228</v>
       </c>
@@ -3353,7 +3396,7 @@
       </c>
       <c r="AA48" s="4"/>
     </row>
-    <row r="49" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>229</v>
       </c>
@@ -3409,7 +3452,7 @@
       </c>
       <c r="AA49" s="4"/>
     </row>
-    <row r="50" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>223</v>
       </c>
@@ -3423,15 +3466,18 @@
         <v>153</v>
       </c>
       <c r="F50" t="s">
-        <v>260</v>
-      </c>
-      <c r="G50" t="s">
-        <v>260</v>
-      </c>
-      <c r="H50" t="s">
-        <v>260</v>
-      </c>
-      <c r="J50" s="3"/>
+        <v>282</v>
+      </c>
+      <c r="G50" t="b">
+        <v>1</v>
+      </c>
+      <c r="H50" t="b">
+        <v>1</v>
+      </c>
+      <c r="I50" t="s">
+        <v>278</v>
+      </c>
+      <c r="J50" s="4"/>
       <c r="K50" t="s">
         <v>234</v>
       </c>
@@ -3462,7 +3508,7 @@
       </c>
       <c r="AA50" s="4"/>
     </row>
-    <row r="51" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>226</v>
       </c>
@@ -3505,7 +3551,7 @@
       </c>
       <c r="T51" s="4"/>
     </row>
-    <row r="52" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>223</v>
       </c>
@@ -3519,15 +3565,18 @@
         <v>153</v>
       </c>
       <c r="F52" t="s">
-        <v>260</v>
-      </c>
-      <c r="G52" t="s">
-        <v>260</v>
-      </c>
-      <c r="H52" t="s">
-        <v>260</v>
-      </c>
-      <c r="J52" s="3"/>
+        <v>282</v>
+      </c>
+      <c r="G52" t="b">
+        <v>0</v>
+      </c>
+      <c r="H52" t="b">
+        <v>0</v>
+      </c>
+      <c r="I52" t="s">
+        <v>278</v>
+      </c>
+      <c r="J52" s="4"/>
       <c r="K52" t="s">
         <v>236</v>
       </c>
@@ -3558,7 +3607,7 @@
       </c>
       <c r="AA52" s="4"/>
     </row>
-    <row r="53" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>223</v>
       </c>
@@ -3572,15 +3621,18 @@
         <v>153</v>
       </c>
       <c r="F53" t="s">
-        <v>260</v>
-      </c>
-      <c r="G53" t="s">
-        <v>260</v>
-      </c>
-      <c r="H53" t="s">
-        <v>260</v>
-      </c>
-      <c r="J53" s="3"/>
+        <v>282</v>
+      </c>
+      <c r="G53" t="b">
+        <v>0</v>
+      </c>
+      <c r="H53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I53" t="s">
+        <v>278</v>
+      </c>
+      <c r="J53" s="4"/>
       <c r="K53" t="s">
         <v>238</v>
       </c>
@@ -3611,7 +3663,7 @@
       </c>
       <c r="AA53" s="4"/>
     </row>
-    <row r="54" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>219</v>
       </c>
@@ -3625,15 +3677,18 @@
         <v>153</v>
       </c>
       <c r="F54" t="s">
-        <v>260</v>
-      </c>
-      <c r="G54" t="s">
-        <v>260</v>
-      </c>
-      <c r="H54" t="s">
-        <v>260</v>
-      </c>
-      <c r="J54" s="3"/>
+        <v>282</v>
+      </c>
+      <c r="G54" t="b">
+        <v>0</v>
+      </c>
+      <c r="H54" t="b">
+        <v>0</v>
+      </c>
+      <c r="I54" t="s">
+        <v>278</v>
+      </c>
+      <c r="J54" s="4"/>
       <c r="K54" t="s">
         <v>240</v>
       </c>
@@ -3664,7 +3719,7 @@
       </c>
       <c r="AA54" s="4"/>
     </row>
-    <row r="55" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>220</v>
       </c>
@@ -3720,7 +3775,7 @@
       </c>
       <c r="AA55" s="4"/>
     </row>
-    <row r="56" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>223</v>
       </c>
@@ -3734,15 +3789,18 @@
         <v>153</v>
       </c>
       <c r="F56" t="s">
-        <v>260</v>
-      </c>
-      <c r="G56" t="s">
-        <v>260</v>
-      </c>
-      <c r="H56" t="s">
-        <v>260</v>
-      </c>
-      <c r="J56" s="3"/>
+        <v>282</v>
+      </c>
+      <c r="G56" t="b">
+        <v>0</v>
+      </c>
+      <c r="H56" t="b">
+        <v>0</v>
+      </c>
+      <c r="I56" t="s">
+        <v>278</v>
+      </c>
+      <c r="J56" s="4"/>
       <c r="K56" t="s">
         <v>242</v>
       </c>
@@ -3773,7 +3831,7 @@
       </c>
       <c r="AA56" s="4"/>
     </row>
-    <row r="57" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>244</v>
       </c>
@@ -3829,7 +3887,7 @@
       </c>
       <c r="AA57" s="4"/>
     </row>
-    <row r="58" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>245</v>
       </c>
@@ -3872,7 +3930,7 @@
       </c>
       <c r="AA58" s="4"/>
     </row>
-    <row r="59" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>248</v>
       </c>
@@ -3915,7 +3973,7 @@
       </c>
       <c r="AA59" s="4"/>
     </row>
-    <row r="60" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>247</v>
       </c>
@@ -3968,7 +4026,7 @@
       </c>
       <c r="AA60" s="4"/>
     </row>
-    <row r="61" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>246</v>
       </c>
@@ -4021,7 +4079,7 @@
       </c>
       <c r="AA61" s="4"/>
     </row>
-    <row r="62" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>250</v>
       </c>
@@ -4061,7 +4119,7 @@
       </c>
       <c r="AA62" s="4"/>
     </row>
-    <row r="63" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>251</v>
       </c>
@@ -4101,7 +4159,7 @@
       </c>
       <c r="AA63" s="4"/>
     </row>
-    <row r="64" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>249</v>
       </c>
@@ -4128,7 +4186,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="65" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>252</v>
       </c>
@@ -4181,7 +4239,7 @@
       </c>
       <c r="AA65" s="4"/>
     </row>
-    <row r="66" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
         <v>253</v>
       </c>
@@ -4234,7 +4292,7 @@
       </c>
       <c r="AA66" s="4"/>
     </row>
-    <row r="67" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>254</v>
       </c>
@@ -4287,7 +4345,7 @@
       </c>
       <c r="AA67" s="4"/>
     </row>
-    <row r="68" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
         <v>255</v>
       </c>
@@ -4340,7 +4398,7 @@
       </c>
       <c r="AA68" s="4"/>
     </row>
-    <row r="69" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>256</v>
       </c>
@@ -4393,7 +4451,7 @@
       </c>
       <c r="AA69" s="4"/>
     </row>
-    <row r="70" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:27" x14ac:dyDescent="0.3">
       <c r="P70" t="s">
         <v>18</v>
       </c>
@@ -4421,7 +4479,7 @@
       </c>
       <c r="AA70" s="4"/>
     </row>
-    <row r="71" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:27" x14ac:dyDescent="0.3">
       <c r="P71" t="s">
         <v>18</v>
       </c>
@@ -4449,7 +4507,7 @@
       </c>
       <c r="AA71" s="4"/>
     </row>
-    <row r="72" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:27" x14ac:dyDescent="0.3">
       <c r="P72" t="s">
         <v>18</v>
       </c>
@@ -4477,7 +4535,7 @@
       </c>
       <c r="AA72" s="4"/>
     </row>
-    <row r="73" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:27" x14ac:dyDescent="0.3">
       <c r="P73" t="s">
         <v>18</v>
       </c>
@@ -4505,7 +4563,7 @@
       </c>
       <c r="AA73" s="4"/>
     </row>
-    <row r="74" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:27" x14ac:dyDescent="0.3">
       <c r="P74" t="s">
         <v>18</v>
       </c>
@@ -4533,7 +4591,7 @@
       </c>
       <c r="AA74" s="4"/>
     </row>
-    <row r="75" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:27" x14ac:dyDescent="0.3">
       <c r="W75" t="s">
         <v>19</v>
       </c>
@@ -4548,7 +4606,7 @@
       </c>
       <c r="AA75" s="4"/>
     </row>
-    <row r="76" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:27" x14ac:dyDescent="0.3">
       <c r="P76" t="s">
         <v>19</v>
       </c>
@@ -4576,7 +4634,7 @@
       </c>
       <c r="AA76" s="4"/>
     </row>
-    <row r="77" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:27" x14ac:dyDescent="0.3">
       <c r="P77" t="s">
         <v>19</v>
       </c>
@@ -4591,7 +4649,7 @@
       </c>
       <c r="T77" s="4"/>
     </row>
-    <row r="78" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:27" x14ac:dyDescent="0.3">
       <c r="P78" t="s">
         <v>19</v>
       </c>
@@ -4619,7 +4677,7 @@
       </c>
       <c r="AA78" s="4"/>
     </row>
-    <row r="79" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:27" x14ac:dyDescent="0.3">
       <c r="P79" t="s">
         <v>19</v>
       </c>
@@ -4647,7 +4705,7 @@
       </c>
       <c r="AA79" s="4"/>
     </row>
-    <row r="80" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:27" x14ac:dyDescent="0.3">
       <c r="P80" t="s">
         <v>19</v>
       </c>
@@ -4675,7 +4733,7 @@
       </c>
       <c r="AA80" s="4"/>
     </row>
-    <row r="81" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="81" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P81" t="s">
         <v>19</v>
       </c>
@@ -4703,7 +4761,7 @@
       </c>
       <c r="AA81" s="4"/>
     </row>
-    <row r="82" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="82" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P82" t="s">
         <v>19</v>
       </c>
@@ -4731,7 +4789,7 @@
       </c>
       <c r="AA82" s="4"/>
     </row>
-    <row r="83" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="83" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P83" t="s">
         <v>19</v>
       </c>
@@ -4759,7 +4817,7 @@
       </c>
       <c r="AA83" s="4"/>
     </row>
-    <row r="84" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="84" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P84" t="s">
         <v>19</v>
       </c>
@@ -4787,7 +4845,7 @@
       </c>
       <c r="AA84" s="4"/>
     </row>
-    <row r="85" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="85" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P85" t="s">
         <v>19</v>
       </c>
@@ -4815,7 +4873,7 @@
       </c>
       <c r="AA85" s="4"/>
     </row>
-    <row r="86" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="86" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P86" t="s">
         <v>19</v>
       </c>
@@ -4843,7 +4901,7 @@
       </c>
       <c r="AA86" s="4"/>
     </row>
-    <row r="87" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="87" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P87" t="s">
         <v>19</v>
       </c>
@@ -4871,7 +4929,7 @@
       </c>
       <c r="AA87" s="4"/>
     </row>
-    <row r="88" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="88" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P88" t="s">
         <v>19</v>
       </c>
@@ -4899,7 +4957,7 @@
       </c>
       <c r="AA88" s="4"/>
     </row>
-    <row r="89" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="89" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P89" t="s">
         <v>19</v>
       </c>
@@ -4927,7 +4985,7 @@
       </c>
       <c r="AA89" s="4"/>
     </row>
-    <row r="90" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="90" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P90" t="s">
         <v>19</v>
       </c>
@@ -4942,7 +5000,7 @@
       </c>
       <c r="T90" s="4"/>
     </row>
-    <row r="91" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="91" spans="16:27" x14ac:dyDescent="0.3">
       <c r="W91" t="s">
         <v>21</v>
       </c>
@@ -4957,7 +5015,7 @@
       </c>
       <c r="AA91" s="4"/>
     </row>
-    <row r="92" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="92" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P92" t="s">
         <v>0</v>
       </c>
@@ -4985,7 +5043,7 @@
       </c>
       <c r="AA92" s="4"/>
     </row>
-    <row r="93" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="93" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P93" t="s">
         <v>0</v>
       </c>
@@ -5013,7 +5071,7 @@
       </c>
       <c r="AA93" s="4"/>
     </row>
-    <row r="94" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="94" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P94" t="s">
         <v>0</v>
       </c>
@@ -5041,7 +5099,7 @@
       </c>
       <c r="AA94" s="4"/>
     </row>
-    <row r="95" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="95" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P95" t="s">
         <v>0</v>
       </c>
@@ -5069,7 +5127,7 @@
       </c>
       <c r="AA95" s="4"/>
     </row>
-    <row r="96" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="96" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P96" t="s">
         <v>0</v>
       </c>
@@ -5097,7 +5155,7 @@
       </c>
       <c r="AA96" s="4"/>
     </row>
-    <row r="97" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="97" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P97" t="s">
         <v>0</v>
       </c>
@@ -5125,7 +5183,7 @@
       </c>
       <c r="AA97" s="4"/>
     </row>
-    <row r="98" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="98" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P98" t="s">
         <v>0</v>
       </c>
@@ -5153,7 +5211,7 @@
       </c>
       <c r="AA98" s="4"/>
     </row>
-    <row r="99" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="99" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P99" t="s">
         <v>0</v>
       </c>
@@ -5181,7 +5239,7 @@
       </c>
       <c r="AA99" s="4"/>
     </row>
-    <row r="100" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="100" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P100" t="s">
         <v>0</v>
       </c>
@@ -5209,7 +5267,7 @@
       </c>
       <c r="AA100" s="4"/>
     </row>
-    <row r="101" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="101" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P101" t="s">
         <v>0</v>
       </c>
@@ -5237,7 +5295,7 @@
       </c>
       <c r="AA101" s="4"/>
     </row>
-    <row r="102" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="102" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P102" t="s">
         <v>0</v>
       </c>
@@ -5265,7 +5323,7 @@
       </c>
       <c r="AA102" s="4"/>
     </row>
-    <row r="103" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="103" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P103" t="s">
         <v>0</v>
       </c>
@@ -5280,7 +5338,7 @@
       </c>
       <c r="T103" s="4"/>
     </row>
-    <row r="104" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="104" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P104" t="s">
         <v>0</v>
       </c>
@@ -5308,7 +5366,7 @@
       </c>
       <c r="AA104" s="4"/>
     </row>
-    <row r="105" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="105" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P105" t="s">
         <v>0</v>
       </c>
@@ -5336,7 +5394,7 @@
       </c>
       <c r="AA105" s="4"/>
     </row>
-    <row r="106" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="106" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P106" t="s">
         <v>0</v>
       </c>
@@ -5364,7 +5422,7 @@
       </c>
       <c r="AA106" s="4"/>
     </row>
-    <row r="107" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="107" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P107" t="s">
         <v>0</v>
       </c>
@@ -5392,7 +5450,7 @@
       </c>
       <c r="AA107" s="4"/>
     </row>
-    <row r="108" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="108" spans="16:27" x14ac:dyDescent="0.3">
       <c r="W108" t="s">
         <v>23</v>
       </c>
@@ -5407,7 +5465,7 @@
       </c>
       <c r="AA108" s="4"/>
     </row>
-    <row r="109" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="109" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P109" t="s">
         <v>21</v>
       </c>
@@ -5435,7 +5493,7 @@
       </c>
       <c r="AA109" s="4"/>
     </row>
-    <row r="110" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="110" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P110" t="s">
         <v>21</v>
       </c>
@@ -5463,7 +5521,7 @@
       </c>
       <c r="AA110" s="4"/>
     </row>
-    <row r="111" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="111" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P111" t="s">
         <v>21</v>
       </c>
@@ -5491,7 +5549,7 @@
       </c>
       <c r="AA111" s="4"/>
     </row>
-    <row r="112" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="112" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P112" t="s">
         <v>21</v>
       </c>
@@ -5519,7 +5577,7 @@
       </c>
       <c r="AA112" s="4"/>
     </row>
-    <row r="113" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="113" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P113" t="s">
         <v>21</v>
       </c>
@@ -5547,7 +5605,7 @@
       </c>
       <c r="AA113" s="4"/>
     </row>
-    <row r="114" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="114" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P114" t="s">
         <v>21</v>
       </c>
@@ -5575,7 +5633,7 @@
       </c>
       <c r="AA114" s="4"/>
     </row>
-    <row r="115" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="115" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P115" t="s">
         <v>21</v>
       </c>
@@ -5603,7 +5661,7 @@
       </c>
       <c r="AA115" s="4"/>
     </row>
-    <row r="116" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="116" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P116" t="s">
         <v>21</v>
       </c>
@@ -5618,7 +5676,7 @@
       </c>
       <c r="T116" s="4"/>
     </row>
-    <row r="117" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="117" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P117" t="s">
         <v>21</v>
       </c>
@@ -5646,7 +5704,7 @@
       </c>
       <c r="AA117" s="4"/>
     </row>
-    <row r="118" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="118" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P118" t="s">
         <v>21</v>
       </c>
@@ -5674,7 +5732,7 @@
       </c>
       <c r="AA118" s="4"/>
     </row>
-    <row r="119" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="119" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P119" t="s">
         <v>21</v>
       </c>
@@ -5702,7 +5760,7 @@
       </c>
       <c r="AA119" s="4"/>
     </row>
-    <row r="120" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="120" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P120" t="s">
         <v>21</v>
       </c>
@@ -5730,7 +5788,7 @@
       </c>
       <c r="AA120" s="4"/>
     </row>
-    <row r="121" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="121" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P121" t="s">
         <v>21</v>
       </c>
@@ -5758,7 +5816,7 @@
       </c>
       <c r="AA121" s="4"/>
     </row>
-    <row r="122" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="122" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P122" t="s">
         <v>21</v>
       </c>
@@ -5786,7 +5844,7 @@
       </c>
       <c r="AA122" s="4"/>
     </row>
-    <row r="123" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="123" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P123" t="s">
         <v>21</v>
       </c>
@@ -5814,7 +5872,7 @@
       </c>
       <c r="AA123" s="4"/>
     </row>
-    <row r="124" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="124" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P124" t="s">
         <v>21</v>
       </c>
@@ -5842,7 +5900,7 @@
       </c>
       <c r="AA124" s="4"/>
     </row>
-    <row r="125" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="125" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P125" t="s">
         <v>21</v>
       </c>
@@ -5870,7 +5928,7 @@
       </c>
       <c r="AA125" s="4"/>
     </row>
-    <row r="126" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="126" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P126" t="s">
         <v>21</v>
       </c>
@@ -5898,7 +5956,7 @@
       </c>
       <c r="AA126" s="4"/>
     </row>
-    <row r="127" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="127" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P127" t="s">
         <v>21</v>
       </c>
@@ -5926,7 +5984,7 @@
       </c>
       <c r="AA127" s="4"/>
     </row>
-    <row r="128" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="128" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P128" t="s">
         <v>21</v>
       </c>
@@ -5954,7 +6012,7 @@
       </c>
       <c r="AA128" s="4"/>
     </row>
-    <row r="129" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="129" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P129" t="s">
         <v>21</v>
       </c>
@@ -5969,7 +6027,7 @@
       </c>
       <c r="T129" s="4"/>
     </row>
-    <row r="130" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="130" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P130" t="s">
         <v>21</v>
       </c>
@@ -5997,7 +6055,7 @@
       </c>
       <c r="AA130" s="4"/>
     </row>
-    <row r="131" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="131" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P131" t="s">
         <v>21</v>
       </c>
@@ -6025,7 +6083,7 @@
       </c>
       <c r="AA131" s="4"/>
     </row>
-    <row r="132" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="132" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P132" t="s">
         <v>21</v>
       </c>
@@ -6053,7 +6111,7 @@
       </c>
       <c r="AA132" s="4"/>
     </row>
-    <row r="133" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="133" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P133" t="s">
         <v>21</v>
       </c>
@@ -6081,7 +6139,7 @@
       </c>
       <c r="AA133" s="4"/>
     </row>
-    <row r="134" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="134" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P134" t="s">
         <v>21</v>
       </c>
@@ -6109,7 +6167,7 @@
       </c>
       <c r="AA134" s="4"/>
     </row>
-    <row r="135" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="135" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P135" t="s">
         <v>21</v>
       </c>
@@ -6137,7 +6195,7 @@
       </c>
       <c r="AA135" s="4"/>
     </row>
-    <row r="136" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="136" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P136" t="s">
         <v>21</v>
       </c>
@@ -6165,7 +6223,7 @@
       </c>
       <c r="AA136" s="4"/>
     </row>
-    <row r="137" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="137" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P137" t="s">
         <v>21</v>
       </c>
@@ -6193,7 +6251,7 @@
       </c>
       <c r="AA137" s="4"/>
     </row>
-    <row r="138" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="138" spans="16:27" x14ac:dyDescent="0.3">
       <c r="W138" t="s">
         <v>40</v>
       </c>
@@ -6208,7 +6266,7 @@
       </c>
       <c r="AA138" s="4"/>
     </row>
-    <row r="139" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="139" spans="16:27" x14ac:dyDescent="0.3">
       <c r="W139" t="s">
         <v>40</v>
       </c>
@@ -6223,7 +6281,7 @@
       </c>
       <c r="AA139" s="4"/>
     </row>
-    <row r="140" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="140" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P140" t="s">
         <v>3</v>
       </c>
@@ -6241,7 +6299,7 @@
       </c>
       <c r="AA140" s="4"/>
     </row>
-    <row r="141" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="141" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P141" t="s">
         <v>144</v>
       </c>
@@ -6262,7 +6320,7 @@
       </c>
       <c r="AA141" s="4"/>
     </row>
-    <row r="142" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="142" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P142" t="s">
         <v>145</v>
       </c>
@@ -6270,7 +6328,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="143" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P143" t="b">
         <v>1</v>
       </c>
@@ -6291,7 +6349,7 @@
       </c>
       <c r="AA143" s="4"/>
     </row>
-    <row r="144" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="144" spans="16:27" x14ac:dyDescent="0.3">
       <c r="W144" t="s">
         <v>41</v>
       </c>
@@ -6306,7 +6364,7 @@
       </c>
       <c r="AA144" s="4"/>
     </row>
-    <row r="145" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="145" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P145" t="s">
         <v>55</v>
       </c>
@@ -6324,7 +6382,7 @@
       </c>
       <c r="AA145" s="4"/>
     </row>
-    <row r="146" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="146" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P146" t="s">
         <v>146</v>
       </c>
@@ -6345,7 +6403,7 @@
       </c>
       <c r="AA146" s="4"/>
     </row>
-    <row r="147" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="147" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P147" t="s">
         <v>1</v>
       </c>
@@ -6366,7 +6424,7 @@
       </c>
       <c r="AA147" s="4"/>
     </row>
-    <row r="148" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="148" spans="16:27" x14ac:dyDescent="0.3">
       <c r="P148" t="b">
         <v>1</v>
       </c>
@@ -6387,7 +6445,7 @@
       </c>
       <c r="AA148" s="4"/>
     </row>
-    <row r="149" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="149" spans="16:27" x14ac:dyDescent="0.3">
       <c r="W149" t="s">
         <v>41</v>
       </c>
@@ -6402,7 +6460,7 @@
       </c>
       <c r="AA149" s="4"/>
     </row>
-    <row r="150" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="150" spans="16:27" x14ac:dyDescent="0.3">
       <c r="W150" t="s">
         <v>41</v>
       </c>
@@ -6417,7 +6475,7 @@
       </c>
       <c r="AA150" s="4"/>
     </row>
-    <row r="151" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="151" spans="16:27" x14ac:dyDescent="0.3">
       <c r="W151" t="s">
         <v>41</v>
       </c>
@@ -6432,7 +6490,7 @@
       </c>
       <c r="AA151" s="4"/>
     </row>
-    <row r="152" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="152" spans="16:27" x14ac:dyDescent="0.3">
       <c r="W152" t="s">
         <v>41</v>
       </c>
@@ -6447,7 +6505,7 @@
       </c>
       <c r="AA152" s="4"/>
     </row>
-    <row r="153" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="153" spans="16:27" x14ac:dyDescent="0.3">
       <c r="W153" t="s">
         <v>41</v>
       </c>
@@ -6462,7 +6520,7 @@
       </c>
       <c r="AA153" s="4"/>
     </row>
-    <row r="154" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="154" spans="16:27" x14ac:dyDescent="0.3">
       <c r="W154" t="s">
         <v>41</v>
       </c>
@@ -6477,7 +6535,7 @@
       </c>
       <c r="AA154" s="4"/>
     </row>
-    <row r="156" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="156" spans="16:27" x14ac:dyDescent="0.3">
       <c r="W156" t="s">
         <v>42</v>
       </c>
@@ -6492,7 +6550,7 @@
       </c>
       <c r="AA156" s="4"/>
     </row>
-    <row r="157" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="157" spans="16:27" x14ac:dyDescent="0.3">
       <c r="W157" t="s">
         <v>42</v>
       </c>
@@ -6507,7 +6565,7 @@
       </c>
       <c r="AA157" s="4"/>
     </row>
-    <row r="158" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="158" spans="16:27" x14ac:dyDescent="0.3">
       <c r="W158" t="s">
         <v>42</v>
       </c>
@@ -6522,7 +6580,7 @@
       </c>
       <c r="AA158" s="4"/>
     </row>
-    <row r="159" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="159" spans="16:27" x14ac:dyDescent="0.3">
       <c r="W159" t="s">
         <v>42</v>
       </c>
@@ -6537,7 +6595,7 @@
       </c>
       <c r="AA159" s="4"/>
     </row>
-    <row r="160" spans="16:27" x14ac:dyDescent="0.25">
+    <row r="160" spans="16:27" x14ac:dyDescent="0.3">
       <c r="W160" t="s">
         <v>42</v>
       </c>
@@ -6552,7 +6610,7 @@
       </c>
       <c r="AA160" s="4"/>
     </row>
-    <row r="161" spans="23:27" x14ac:dyDescent="0.25">
+    <row r="161" spans="23:27" x14ac:dyDescent="0.3">
       <c r="W161" t="s">
         <v>42</v>
       </c>
@@ -6567,7 +6625,7 @@
       </c>
       <c r="AA161" s="4"/>
     </row>
-    <row r="162" spans="23:27" x14ac:dyDescent="0.25">
+    <row r="162" spans="23:27" x14ac:dyDescent="0.3">
       <c r="W162" t="s">
         <v>42</v>
       </c>
@@ -6582,7 +6640,7 @@
       </c>
       <c r="AA162" s="4"/>
     </row>
-    <row r="163" spans="23:27" x14ac:dyDescent="0.25">
+    <row r="163" spans="23:27" x14ac:dyDescent="0.3">
       <c r="W163" t="s">
         <v>42</v>
       </c>
@@ -6597,7 +6655,7 @@
       </c>
       <c r="AA163" s="4"/>
     </row>
-    <row r="164" spans="23:27" x14ac:dyDescent="0.25">
+    <row r="164" spans="23:27" x14ac:dyDescent="0.3">
       <c r="W164" t="s">
         <v>42</v>
       </c>
@@ -6612,7 +6670,7 @@
       </c>
       <c r="AA164" s="4"/>
     </row>
-    <row r="165" spans="23:27" x14ac:dyDescent="0.25">
+    <row r="165" spans="23:27" x14ac:dyDescent="0.3">
       <c r="W165" t="s">
         <v>42</v>
       </c>
@@ -6627,7 +6685,7 @@
       </c>
       <c r="AA165" s="4"/>
     </row>
-    <row r="166" spans="23:27" x14ac:dyDescent="0.25">
+    <row r="166" spans="23:27" x14ac:dyDescent="0.3">
       <c r="W166" t="s">
         <v>42</v>
       </c>
@@ -6642,7 +6700,7 @@
       </c>
       <c r="AA166" s="4"/>
     </row>
-    <row r="167" spans="23:27" x14ac:dyDescent="0.25">
+    <row r="167" spans="23:27" x14ac:dyDescent="0.3">
       <c r="W167" t="s">
         <v>42</v>
       </c>
@@ -6657,7 +6715,7 @@
       </c>
       <c r="AA167" s="4"/>
     </row>
-    <row r="169" spans="23:27" x14ac:dyDescent="0.25">
+    <row r="169" spans="23:27" x14ac:dyDescent="0.3">
       <c r="W169" t="s">
         <v>43</v>
       </c>
@@ -6672,7 +6730,7 @@
       </c>
       <c r="AA169" s="4"/>
     </row>
-    <row r="170" spans="23:27" x14ac:dyDescent="0.25">
+    <row r="170" spans="23:27" x14ac:dyDescent="0.3">
       <c r="W170" t="s">
         <v>43</v>
       </c>
@@ -6687,7 +6745,7 @@
       </c>
       <c r="AA170" s="4"/>
     </row>
-    <row r="171" spans="23:27" x14ac:dyDescent="0.25">
+    <row r="171" spans="23:27" x14ac:dyDescent="0.3">
       <c r="W171" t="s">
         <v>43</v>
       </c>
@@ -6702,7 +6760,7 @@
       </c>
       <c r="AA171" s="4"/>
     </row>
-    <row r="172" spans="23:27" x14ac:dyDescent="0.25">
+    <row r="172" spans="23:27" x14ac:dyDescent="0.3">
       <c r="W172" t="s">
         <v>43</v>
       </c>
@@ -6717,7 +6775,7 @@
       </c>
       <c r="AA172" s="4"/>
     </row>
-    <row r="173" spans="23:27" x14ac:dyDescent="0.25">
+    <row r="173" spans="23:27" x14ac:dyDescent="0.3">
       <c r="W173" t="s">
         <v>43</v>
       </c>
@@ -6732,7 +6790,7 @@
       </c>
       <c r="AA173" s="4"/>
     </row>
-    <row r="174" spans="23:27" x14ac:dyDescent="0.25">
+    <row r="174" spans="23:27" x14ac:dyDescent="0.3">
       <c r="W174" t="s">
         <v>43</v>
       </c>
@@ -6747,7 +6805,7 @@
       </c>
       <c r="AA174" s="4"/>
     </row>
-    <row r="175" spans="23:27" x14ac:dyDescent="0.25">
+    <row r="175" spans="23:27" x14ac:dyDescent="0.3">
       <c r="W175" t="s">
         <v>43</v>
       </c>
@@ -6762,7 +6820,7 @@
       </c>
       <c r="AA175" s="4"/>
     </row>
-    <row r="176" spans="23:27" x14ac:dyDescent="0.25">
+    <row r="176" spans="23:27" x14ac:dyDescent="0.3">
       <c r="W176" t="s">
         <v>43</v>
       </c>
@@ -6777,7 +6835,7 @@
       </c>
       <c r="AA176" s="4"/>
     </row>
-    <row r="177" spans="23:27" x14ac:dyDescent="0.25">
+    <row r="177" spans="23:27" x14ac:dyDescent="0.3">
       <c r="W177" t="s">
         <v>43</v>
       </c>
@@ -6792,7 +6850,7 @@
       </c>
       <c r="AA177" s="4"/>
     </row>
-    <row r="178" spans="23:27" x14ac:dyDescent="0.25">
+    <row r="178" spans="23:27" x14ac:dyDescent="0.3">
       <c r="W178" t="s">
         <v>43</v>
       </c>
@@ -6807,7 +6865,7 @@
       </c>
       <c r="AA178" s="4"/>
     </row>
-    <row r="179" spans="23:27" x14ac:dyDescent="0.25">
+    <row r="179" spans="23:27" x14ac:dyDescent="0.3">
       <c r="W179" t="s">
         <v>43</v>
       </c>
@@ -6822,7 +6880,7 @@
       </c>
       <c r="AA179" s="4"/>
     </row>
-    <row r="180" spans="23:27" x14ac:dyDescent="0.25">
+    <row r="180" spans="23:27" x14ac:dyDescent="0.3">
       <c r="W180" t="s">
         <v>43</v>
       </c>
@@ -6855,14 +6913,14 @@
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
       <c r="F6" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>88</v>
       </c>
@@ -6888,7 +6946,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>102</v>
       </c>
@@ -6914,7 +6972,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>103</v>
       </c>
@@ -6940,7 +6998,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>104</v>
       </c>
@@ -6966,7 +7024,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>96</v>
       </c>
@@ -6992,7 +7050,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>105</v>
       </c>
@@ -7018,7 +7076,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>106</v>
       </c>
@@ -7044,7 +7102,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>107</v>
       </c>
@@ -7070,7 +7128,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F17" t="s">
         <v>109</v>
       </c>

</xml_diff>